<commit_message>
2022Q4 DCF Update for TexasInstruments (TXN)
Pretty fairly valued.
Price target: $146.82
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8286BEED-E7FC-4AA1-854B-45460362F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449E3FC8-7E83-455B-9B6B-289593E193ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23520" yWindow="2820" windowWidth="26730" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="18030" yWindow="4650" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comm Ind Bld Spply" sheetId="1" r:id="rId1"/>
+    <sheet name="WatchList" sheetId="1" r:id="rId1"/>
     <sheet name="Semiconductors" sheetId="3" r:id="rId2"/>
     <sheet name="Clothing" sheetId="2" r:id="rId3"/>
     <sheet name="Etc." sheetId="4" r:id="rId4"/>
@@ -39,6 +39,7 @@
     <externalReference r:id="rId22"/>
     <externalReference r:id="rId23"/>
     <externalReference r:id="rId24"/>
+    <externalReference r:id="rId25"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>Ticker</t>
   </si>
@@ -428,16 +429,32 @@
   </si>
   <si>
     <t>Cruise liner, exploration</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Semiconductors</t>
+  </si>
+  <si>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>EBITDA/Sh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -526,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -587,6 +604,12 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,150 +775,6 @@
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -913,28 +792,34 @@
         </row>
         <row r="9">
           <cell r="N9">
-            <v>42159.523249999998</v>
+            <v>41885.595249999998</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>17804.335737361998</v>
+            <v>17718.474111348907</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>69.801489535705741</v>
+            <v>69.464871001991241</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1">
+        <row r="27">
+          <cell r="AA27">
+            <v>642.59899999999948</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -968,14 +853,20 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1">
+        <row r="27">
+          <cell r="Z27">
+            <v>-2103</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1010,7 +901,156 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Dash"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="N4">
+            <v>11.68</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="N9">
+            <v>1089.1226000000001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>473.84250172820322</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>8.932840074054166</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>67.2</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>87517.207200000004</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>74903.518611460153</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>63.631730278242067</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="O3">
+            <v>18.149999999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="O8">
+            <v>506.71814999999992</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="O18">
+            <v>541.46267091390234</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="O19">
+            <v>16.629178185986376</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>4.43</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>217.09325999999999</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>42.225188935657137</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>0.9450156424434254</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1055,6 +1095,42 @@
 <file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
@@ -1065,29 +1141,35 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="4">
-          <cell r="N4">
-            <v>11.68</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="N9">
-            <v>1089.1226000000001</v>
+        <row r="5">
+          <cell r="N5">
+            <v>169.8</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>156055.80000000002</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>473.84250172820322</v>
+            <v>134489.60313830531</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>8.932840074054166</v>
+            <v>146.82271084967829</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="X28">
+            <v>11119</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1642,11 +1724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1654,19 +1736,21 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1677,13 +1761,13 @@
         <v>81</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>80</v>
@@ -1694,20 +1778,29 @@
       <c r="I1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1717,14 +1810,14 @@
       <c r="C2" s="4">
         <v>44775</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
       </c>
       <c r="G2" s="22">
         <v>44775</v>
@@ -1737,23 +1830,23 @@
         <f>[1]Main!$N$19</f>
         <v>22198.677928000903</v>
       </c>
-      <c r="J2" s="19">
+      <c r="M2" s="19">
         <f>[1]Main!$N$3</f>
         <v>107</v>
       </c>
-      <c r="K2" s="19">
+      <c r="N2" s="19">
         <f>[1]Main!$N$20</f>
         <v>506.49669636225735</v>
       </c>
-      <c r="L2" s="14">
-        <f>K2/J2</f>
+      <c r="O2" s="14">
+        <f>N2/M2</f>
         <v>4.733613984693994</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -1763,14 +1856,14 @@
       <c r="C3" s="4">
         <v>44772</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
       </c>
       <c r="G3" s="22">
         <v>44858</v>
@@ -1783,23 +1876,23 @@
         <f>[2]Main!$N$18</f>
         <v>11759.15586027935</v>
       </c>
-      <c r="J3" s="19">
+      <c r="M3" s="19">
         <f>[2]Main!$N$3</f>
         <v>138.47</v>
       </c>
-      <c r="K3" s="19">
+      <c r="N3" s="19">
         <f>[2]Main!$N$19</f>
         <v>605.54899120857669</v>
       </c>
-      <c r="L3" s="14">
-        <f>K3/J3</f>
+      <c r="O3" s="14">
+        <f>N3/M3</f>
         <v>4.3731421333760139</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -1809,14 +1902,14 @@
       <c r="C4" s="4">
         <v>44773</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
       </c>
       <c r="G4" s="22">
         <v>44771</v>
@@ -1829,20 +1922,20 @@
         <f>[3]Main!$N$18</f>
         <v>8817.3705876180775</v>
       </c>
-      <c r="J4" s="19">
+      <c r="M4" s="19">
         <f>[3]Main!$N$3</f>
         <v>35.31</v>
       </c>
-      <c r="K4" s="19">
+      <c r="N4" s="19">
         <f>[3]Main!$N$19</f>
         <v>52.989005935204794</v>
       </c>
-      <c r="L4" s="14">
-        <f t="shared" ref="L4:L17" si="0">K4/J4</f>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O18" si="0">N4/M4</f>
         <v>1.5006798622261339</v>
       </c>
     </row>
-    <row r="5" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -1852,14 +1945,14 @@
       <c r="C5" s="4">
         <v>44773</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>58</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
       </c>
       <c r="G5" s="22">
         <v>44776</v>
@@ -1872,20 +1965,20 @@
         <f>[4]Main!$N$19</f>
         <v>2996.7820265448186</v>
       </c>
-      <c r="J5" s="19">
+      <c r="M5" s="19">
         <f>[4]Main!$N$3</f>
         <v>64.72</v>
       </c>
-      <c r="K5" s="19">
+      <c r="N5" s="19">
         <f>[4]Main!$N$20</f>
         <v>66.876035494517382</v>
       </c>
-      <c r="L5" s="14">
+      <c r="O5" s="14">
         <f t="shared" si="0"/>
         <v>1.0333132801995888</v>
       </c>
     </row>
-    <row r="6" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -1895,14 +1988,14 @@
       <c r="C6" s="4">
         <v>44773</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
       </c>
       <c r="G6" s="22">
         <v>44865</v>
@@ -1915,20 +2008,20 @@
         <f>[5]Main!$N$18</f>
         <v>4076.5725319753483</v>
       </c>
-      <c r="J6" s="19">
+      <c r="M6" s="19">
         <f>[5]Main!$N$3</f>
         <v>87</v>
       </c>
-      <c r="K6" s="19">
+      <c r="N6" s="19">
         <f>[5]Main!$N$19</f>
         <v>436.69397285882815</v>
       </c>
-      <c r="L6" s="14">
+      <c r="O6" s="14">
         <f t="shared" si="0"/>
         <v>5.0194709524003231</v>
       </c>
     </row>
-    <row r="7" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -1938,14 +2031,14 @@
       <c r="C7" s="4">
         <v>44774</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
       </c>
       <c r="G7" s="22">
         <v>44867</v>
@@ -1958,20 +2051,20 @@
         <f>[6]Main!$N$18</f>
         <v>50207.036438406729</v>
       </c>
-      <c r="J7" s="19">
+      <c r="M7" s="19">
         <f>[6]Main!$N$3</f>
         <v>73.459999999999994</v>
       </c>
-      <c r="K7" s="19">
+      <c r="N7" s="19">
         <f>[6]Main!$N$19</f>
         <v>294.64223261975781</v>
       </c>
-      <c r="L7" s="14">
+      <c r="O7" s="14">
         <f t="shared" si="0"/>
         <v>4.0109206727437767</v>
       </c>
     </row>
-    <row r="8" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -1981,14 +2074,14 @@
       <c r="C8" s="4">
         <v>44774</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
       </c>
       <c r="G8" s="22">
         <v>44782</v>
@@ -2001,20 +2094,20 @@
         <f>[7]Main!$N$18</f>
         <v>12229.883434318077</v>
       </c>
-      <c r="J8" s="19">
+      <c r="M8" s="19">
         <f>[7]Main!$N$3</f>
         <v>64.44</v>
       </c>
-      <c r="K8" s="19">
+      <c r="N8" s="19">
         <f>[7]Main!$N$19</f>
         <v>142.2079469106753</v>
       </c>
-      <c r="L8" s="14">
+      <c r="O8" s="14">
         <f t="shared" si="0"/>
         <v>2.2068272332507033</v>
       </c>
     </row>
-    <row r="9" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -2024,14 +2117,14 @@
       <c r="C9" s="4">
         <v>44774</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
       <c r="G9" s="22">
         <v>44804</v>
@@ -2044,20 +2137,20 @@
         <f>[8]Main!$N$18</f>
         <v>1643.4101590621442</v>
       </c>
-      <c r="J9" s="19">
+      <c r="M9" s="19">
         <f>[8]Main!$N$3</f>
         <v>25.18</v>
       </c>
-      <c r="K9" s="19">
+      <c r="N9" s="19">
         <f>[8]Main!$N$19</f>
         <v>49.564500982059428</v>
       </c>
-      <c r="L9" s="14">
+      <c r="O9" s="14">
         <f t="shared" si="0"/>
         <v>1.9684075052446159</v>
       </c>
     </row>
-    <row r="10" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -2067,14 +2160,14 @@
       <c r="C10" s="4">
         <v>44775</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
       </c>
       <c r="G10" s="22">
         <v>44865</v>
@@ -2087,20 +2180,20 @@
         <f>[9]Main!$N$18</f>
         <v>8831.5667844635373</v>
       </c>
-      <c r="J10" s="19">
+      <c r="M10" s="19">
         <f>[9]Main!$N$3</f>
         <v>260.32</v>
       </c>
-      <c r="K10" s="19">
+      <c r="N10" s="19">
         <f>[9]Main!$N$19</f>
         <v>357.06180902658434</v>
       </c>
-      <c r="L10" s="14">
+      <c r="O10" s="14">
         <f t="shared" si="0"/>
         <v>1.3716264944168115</v>
       </c>
     </row>
-    <row r="11" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2110,14 +2203,14 @@
       <c r="C11" s="4">
         <v>44775</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
       </c>
       <c r="G11" s="22">
         <v>44777</v>
@@ -2130,20 +2223,20 @@
         <f>[10]Main!$N$18</f>
         <v>6053.073284927159</v>
       </c>
-      <c r="J11" s="19">
+      <c r="M11" s="19">
         <f>[10]Main!$N$3</f>
         <v>60.73</v>
       </c>
-      <c r="K11" s="19">
+      <c r="N11" s="19">
         <f>[10]Main!$N$19</f>
         <v>86.349119613796859</v>
       </c>
-      <c r="L11" s="14">
-        <f>K11/J11</f>
+      <c r="O11" s="14">
+        <f>N11/M11</f>
         <v>1.4218527846829716</v>
       </c>
     </row>
-    <row r="12" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2153,14 +2246,14 @@
       <c r="C12" s="4">
         <v>44775</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>78</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
       </c>
       <c r="G12" s="22">
         <v>44777</v>
@@ -2173,24 +2266,24 @@
         <f>[11]Main!$N$18</f>
         <v>2666.8844433216959</v>
       </c>
-      <c r="J12" s="19">
+      <c r="M12" s="19">
         <f>[11]Main!$N$3</f>
         <v>20.86</v>
       </c>
-      <c r="K12" s="19">
+      <c r="N12" s="19">
         <f>[11]Main!$N$19</f>
         <v>17.243419112262924</v>
       </c>
-      <c r="L12" s="14">
+      <c r="O12" s="14">
         <f t="shared" si="0"/>
         <v>0.82662603606246043</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
         <v>89</v>
       </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -2200,14 +2293,14 @@
       <c r="C13" s="4">
         <v>44778</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>100</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
       </c>
       <c r="G13" s="22">
         <v>44870</v>
@@ -2220,20 +2313,20 @@
         <f>[12]Main!$N$18</f>
         <v>59674.776053903901</v>
       </c>
-      <c r="J13" s="19">
+      <c r="M13" s="19">
         <f>[12]Main!$N$3</f>
         <v>76.150000000000006</v>
       </c>
-      <c r="K13" s="19">
+      <c r="N13" s="19">
         <f>[12]Main!$N$19</f>
         <v>170.11053607156185</v>
       </c>
-      <c r="L13" s="14">
+      <c r="O13" s="14">
         <f t="shared" si="0"/>
         <v>2.2338875386941806</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -2241,42 +2334,54 @@
         <v>124</v>
       </c>
       <c r="C14" s="4">
-        <v>44972</v>
-      </c>
-      <c r="D14" s="26" t="s">
+        <v>44973</v>
+      </c>
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>120</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
       </c>
       <c r="G14" s="22">
         <v>45049</v>
       </c>
       <c r="H14" s="12">
-        <f>[17]Main!$N$9</f>
-        <v>42159.523249999998</v>
+        <f>[13]Main!$N$9</f>
+        <v>41885.595249999998</v>
       </c>
       <c r="I14" s="13">
-        <f>[17]Main!$N$12</f>
-        <v>17804.335737361998</v>
-      </c>
-      <c r="J14" s="23">
-        <f>[17]Main!$N$4</f>
+        <f>[13]Main!$N$12</f>
+        <v>17718.474111348907</v>
+      </c>
+      <c r="J14" s="13">
+        <f>+[13]Model!$AA$27</f>
+        <v>642.59899999999948</v>
+      </c>
+      <c r="K14" s="29">
+        <f>J14/(I14/N14)</f>
+        <v>2.519294627770305</v>
+      </c>
+      <c r="L14" s="28">
+        <f>H14/J14</f>
+        <v>65.181544400162522</v>
+      </c>
+      <c r="M14" s="19">
+        <f>[13]Main!$N$4</f>
         <v>75.75</v>
       </c>
-      <c r="K14" s="23">
-        <f>[17]Main!$N$13</f>
-        <v>69.801489535705741</v>
-      </c>
-      <c r="L14" s="14">
+      <c r="N14" s="19">
+        <f>[13]Main!$N$13</f>
+        <v>69.464871001991241</v>
+      </c>
+      <c r="O14" s="14">
         <f t="shared" si="0"/>
-        <v>0.92147180905222104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>0.91702800002628704</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2286,40 +2391,52 @@
       <c r="C15" s="4">
         <v>44972</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>119</v>
-      </c>
-      <c r="F15" t="s">
-        <v>123</v>
       </c>
       <c r="G15" s="22">
         <v>45005</v>
       </c>
       <c r="H15" s="12">
-        <f>[18]Main!$N$9</f>
+        <f>[14]Main!$N$9</f>
         <v>43973.122093023252</v>
       </c>
       <c r="I15" s="13">
-        <f>[18]Main!$N$12</f>
+        <f>[14]Main!$N$12</f>
         <v>18848.439289507303</v>
       </c>
-      <c r="J15" s="23">
-        <f>[18]Main!$N$4</f>
+      <c r="J15" s="13">
+        <f>+[14]Model!$Z$27</f>
+        <v>-2103</v>
+      </c>
+      <c r="K15" s="29">
+        <f>J15/(I15/N15)</f>
+        <v>-1.7809748892171344</v>
+      </c>
+      <c r="L15" s="28">
+        <f>H15/J15</f>
+        <v>-20.909710933439491</v>
+      </c>
+      <c r="M15" s="19">
+        <f>[14]Main!$N$4</f>
         <v>12.19</v>
       </c>
-      <c r="K15" s="23">
-        <f>[18]Main!$N$13</f>
+      <c r="N15" s="19">
+        <f>[14]Main!$N$13</f>
         <v>15.962243022133215</v>
       </c>
-      <c r="L15" s="14">
+      <c r="O15" s="14">
         <f t="shared" si="0"/>
         <v>1.3094538984522737</v>
       </c>
     </row>
-    <row r="16" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -2329,40 +2446,51 @@
       <c r="C16" s="4">
         <v>44972</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>121</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
       </c>
       <c r="G16" s="22">
         <v>44985</v>
       </c>
       <c r="H16" s="12">
-        <f>[19]Main!$N$9</f>
+        <f>[15]Main!$N$9</f>
         <v>19478.988389999999</v>
       </c>
       <c r="I16" s="13">
-        <f>[19]Main!$N$12</f>
+        <f>[15]Main!$N$12</f>
         <v>9576.3280554549001</v>
       </c>
-      <c r="J16" s="23">
-        <f>[19]Main!$N$4</f>
+      <c r="J16" s="13">
+        <v>-724</v>
+      </c>
+      <c r="K16" s="29">
+        <f>J16/(I16/N16)</f>
+        <v>-1.9811245892039655</v>
+      </c>
+      <c r="L16" s="28">
+        <f>H16/J16</f>
+        <v>-26.90468009668508</v>
+      </c>
+      <c r="M16" s="19">
+        <f>[15]Main!$N$4</f>
         <v>18.11</v>
       </c>
-      <c r="K16" s="23">
-        <f>[19]Main!$N$13</f>
+      <c r="N16" s="19">
+        <f>[15]Main!$N$13</f>
         <v>26.204280365946822</v>
       </c>
-      <c r="L16" s="14">
+      <c r="O16" s="14">
         <f t="shared" si="0"/>
         <v>1.4469508760876213</v>
       </c>
     </row>
-    <row r="17" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2372,41 +2500,104 @@
       <c r="C17" s="4">
         <v>44972</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>122</v>
-      </c>
-      <c r="F17" t="s">
-        <v>76</v>
       </c>
       <c r="G17" s="22">
         <v>44985</v>
       </c>
       <c r="H17" s="12">
-        <f>[20]Main!$N$9</f>
+        <f>[16]Main!$N$9</f>
         <v>1089.1226000000001</v>
       </c>
       <c r="I17" s="13">
-        <f>[20]Main!$N$12</f>
+        <f>[16]Main!$N$12</f>
         <v>473.84250172820322</v>
       </c>
-      <c r="J17" s="23">
-        <f>[20]Main!$N$4</f>
+      <c r="J17" s="13">
+        <v>2</v>
+      </c>
+      <c r="K17" s="29">
+        <f>J17/(I17/N17)</f>
+        <v>3.7703836365350178E-2</v>
+      </c>
+      <c r="L17" s="28">
+        <f>H17/J17</f>
+        <v>544.56130000000007</v>
+      </c>
+      <c r="M17" s="19">
+        <f>[16]Main!$N$4</f>
         <v>11.68</v>
       </c>
-      <c r="K17" s="23">
-        <f>[20]Main!$N$13</f>
+      <c r="N17" s="19">
+        <f>[16]Main!$N$13</f>
         <v>8.932840074054166</v>
       </c>
-      <c r="L17" s="14">
+      <c r="O17" s="14">
         <f t="shared" si="0"/>
         <v>0.76479795154573338</v>
       </c>
     </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="4">
+        <v>44979</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="12">
+        <f>[21]Main!$N$10</f>
+        <v>156055.80000000002</v>
+      </c>
+      <c r="I18" s="13">
+        <f>[21]Main!$N$12</f>
+        <v>134489.60313830531</v>
+      </c>
+      <c r="J18" s="13">
+        <f>[21]Model!$X$28</f>
+        <v>11119</v>
+      </c>
+      <c r="K18" s="29">
+        <f>J18/(I18/N18)</f>
+        <v>12.138646288209607</v>
+      </c>
+      <c r="L18" s="28">
+        <f>H18/J18</f>
+        <v>14.035057109452291</v>
+      </c>
+      <c r="M18" s="19">
+        <f>[21]Main!$N$5</f>
+        <v>169.8</v>
+      </c>
+      <c r="N18" s="19">
+        <f>[21]Main!$N$13</f>
+        <v>146.82271084967829</v>
+      </c>
+      <c r="O18" s="14">
+        <f>N18/M18</f>
+        <v>0.86468027591094387</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:L1048576">
+  <conditionalFormatting sqref="O1:O1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2419,25 +2610,26 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{73328F8B-1F94-4A8A-9A78-403E164E8CF5}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{9DBC66B9-2FF1-4977-B2DF-8C41D4A7A6D1}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{13EDAF3C-5721-4D75-9703-2DB05A32F554}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{1F57513D-24D3-4658-8F68-AF40A09EFC74}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{7760A594-AEAF-4B58-817B-4761F7B99113}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{F26D788E-1A4C-438C-9388-1DE3F435DDD3}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{C5B7B287-A56A-4BF1-A85C-5D722595DDC9}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{608B7647-1B08-4C9F-9F67-8EE648DE91F4}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{EC971D85-AE4D-4BAC-8F79-E09E5BB1E48F}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{3F8536C2-23A7-4161-812E-20365E1D9978}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{EADEAE13-3EB5-4DD8-A227-962C1710AB1F}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{8891FA92-2D91-4B39-8F9A-15A7A99C6B0E}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{B17BAEAB-F391-4432-AAF4-5E33835BE8BD}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{C1F4114B-46BB-4059-A5BE-C706C0D64BF9}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{6B733B71-6254-4B4B-A709-845BAA354A79}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{8C7CEC3F-9A88-4BF1-8E7D-6185C3B6C9AF}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{73328F8B-1F94-4A8A-9A78-403E164E8CF5}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{9DBC66B9-2FF1-4977-B2DF-8C41D4A7A6D1}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{13EDAF3C-5721-4D75-9703-2DB05A32F554}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{1F57513D-24D3-4658-8F68-AF40A09EFC74}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{7760A594-AEAF-4B58-817B-4761F7B99113}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{F26D788E-1A4C-438C-9388-1DE3F435DDD3}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{C5B7B287-A56A-4BF1-A85C-5D722595DDC9}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{608B7647-1B08-4C9F-9F67-8EE648DE91F4}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{EC971D85-AE4D-4BAC-8F79-E09E5BB1E48F}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{3F8536C2-23A7-4161-812E-20365E1D9978}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{EADEAE13-3EB5-4DD8-A227-962C1710AB1F}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{8891FA92-2D91-4B39-8F9A-15A7A99C6B0E}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{B17BAEAB-F391-4432-AAF4-5E33835BE8BD}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{C1F4114B-46BB-4059-A5BE-C706C0D64BF9}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{6B733B71-6254-4B4B-A709-845BAA354A79}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{8C7CEC3F-9A88-4BF1-8E7D-6185C3B6C9AF}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{0B716ECA-DE4E-45F0-86A2-02472C2F8EAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -2446,7 +2638,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,19 +3067,19 @@
         <v>33</v>
       </c>
       <c r="G6" s="12">
-        <f>+[13]Main!$J$8</f>
+        <f>+[17]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[13]Main!$J$18</f>
+        <f>+[17]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[13]Main!$J$3</f>
+        <f>+[17]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[13]Main!$J$19</f>
+        <f>+[17]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3170,19 +3362,19 @@
         <v>97</v>
       </c>
       <c r="G2" s="12">
-        <f>[14]Main!$O$8</f>
+        <f>[18]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[14]Main!$O$18</f>
+        <f>[18]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[14]Main!$O$3</f>
+        <f>[18]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[14]Main!$O$19</f>
+        <f>[18]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3210,19 +3402,19 @@
         <v>103</v>
       </c>
       <c r="G3" s="12">
-        <f>+[15]Main!$N$8</f>
+        <f>+[19]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[15]Main!$N$18</f>
+        <f>+[19]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[15]Main!$N$3</f>
+        <f>+[19]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[15]Main!$N$19</f>
+        <f>+[19]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3253,19 +3445,19 @@
         <v>108</v>
       </c>
       <c r="G4" s="12">
-        <f>[16]Main!$J$8</f>
+        <f>[20]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[16]Main!$J$18</f>
+        <f>[20]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[16]Main!$J$3</f>
+        <f>[20]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[16]Main!$J$19</f>
+        <f>[20]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2023Q1 DCF Update for AnalogDevices (ADI)
Pretty fairly valued.
Price target: $188.41
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449E3FC8-7E83-455B-9B6B-289593E193ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C06148E-A635-4846-AA21-B2F95C871DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18030" yWindow="4650" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="5070" yWindow="1170" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,7 @@
     <externalReference r:id="rId23"/>
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
+    <externalReference r:id="rId26"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
   <si>
     <t>Ticker</t>
   </si>
@@ -813,7 +814,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -860,7 +861,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -901,7 +902,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -951,34 +952,45 @@
 <file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+        <row r="5">
+          <cell r="N5">
+            <v>169.8</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>156055.80000000002</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>134489.60313830531</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>146.82271084967829</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="X28">
+            <v>11119</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -994,23 +1006,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1030,23 +1042,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1102,23 +1114,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1129,6 +1141,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1143,29 +1191,38 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="N5">
-            <v>169.8</v>
+            <v>185.65</v>
           </cell>
         </row>
         <row r="10">
           <cell r="N10">
-            <v>156055.80000000002</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="N12">
-            <v>134489.60313830531</v>
+            <v>99554.828000000009</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>146.82271084967829</v>
+            <v>95545.612738294119</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>188.40829140695323</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="28">
-          <cell r="X28">
-            <v>11119</v>
+        <row r="29">
+          <cell r="J29">
+            <v>303.0739999999995</v>
+          </cell>
+          <cell r="K29">
+            <v>268.88500000000033</v>
+          </cell>
+          <cell r="L29">
+            <v>472.50999999999863</v>
+          </cell>
+          <cell r="M29">
+            <v>486.34199999999987</v>
           </cell>
         </row>
       </sheetData>
@@ -1724,11 +1781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomLeft" activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1988,7 @@
         <v>52.989005935204794</v>
       </c>
       <c r="O4" s="14">
-        <f t="shared" ref="O4:O18" si="0">N4/M4</f>
+        <f t="shared" ref="O4:O17" si="0">N4/M4</f>
         <v>1.5006798622261339</v>
       </c>
     </row>
@@ -2564,15 +2621,15 @@
         <v>22</v>
       </c>
       <c r="H18" s="12">
-        <f>[21]Main!$N$10</f>
+        <f>[17]Main!$N$10</f>
         <v>156055.80000000002</v>
       </c>
       <c r="I18" s="13">
-        <f>[21]Main!$N$12</f>
+        <f>[17]Main!$N$12</f>
         <v>134489.60313830531</v>
       </c>
       <c r="J18" s="13">
-        <f>[21]Model!$X$28</f>
+        <f>[17]Model!$X$28</f>
         <v>11119</v>
       </c>
       <c r="K18" s="29">
@@ -2584,16 +2641,68 @@
         <v>14.035057109452291</v>
       </c>
       <c r="M18" s="19">
-        <f>[21]Main!$N$5</f>
+        <f>[17]Main!$N$5</f>
         <v>169.8</v>
       </c>
       <c r="N18" s="19">
-        <f>[21]Main!$N$13</f>
+        <f>[17]Main!$N$13</f>
         <v>146.82271084967829</v>
       </c>
       <c r="O18" s="14">
         <f>N18/M18</f>
         <v>0.86468027591094387</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="4">
+        <v>44980</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="12">
+        <f>[22]Main!$N$10</f>
+        <v>99554.828000000009</v>
+      </c>
+      <c r="I19" s="13">
+        <f>+[22]Main!$N$13</f>
+        <v>95545.612738294119</v>
+      </c>
+      <c r="J19" s="13">
+        <f>SUM([22]Model!$J$29:$M$29)</f>
+        <v>1530.8109999999983</v>
+      </c>
+      <c r="K19" s="29">
+        <f>J19/(I19/N19)</f>
+        <v>3.0186366146079791</v>
+      </c>
+      <c r="L19" s="28">
+        <f>H19/J19</f>
+        <v>65.034042739436885</v>
+      </c>
+      <c r="M19" s="19">
+        <f>+[22]Main!$N$5</f>
+        <v>185.65</v>
+      </c>
+      <c r="N19" s="19">
+        <f>+[22]Main!$N$14</f>
+        <v>188.40829140695323</v>
+      </c>
+      <c r="O19" s="14">
+        <f>N19/M19</f>
+        <v>1.0148574813194355</v>
       </c>
     </row>
   </sheetData>
@@ -2627,9 +2736,10 @@
     <hyperlink ref="E16" r:id="rId15" xr:uid="{6B733B71-6254-4B4B-A709-845BAA354A79}"/>
     <hyperlink ref="E17" r:id="rId16" xr:uid="{8C7CEC3F-9A88-4BF1-8E7D-6185C3B6C9AF}"/>
     <hyperlink ref="E18" r:id="rId17" xr:uid="{0B716ECA-DE4E-45F0-86A2-02472C2F8EAB}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{9712A0F2-E276-4023-8E1C-20FFFF3D79AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -2638,7 +2748,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3067,19 +3177,19 @@
         <v>33</v>
       </c>
       <c r="G6" s="12">
-        <f>+[17]Main!$J$8</f>
+        <f>+[18]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[17]Main!$J$18</f>
+        <f>+[18]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[17]Main!$J$3</f>
+        <f>+[18]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[17]Main!$J$19</f>
+        <f>+[18]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3362,19 +3472,19 @@
         <v>97</v>
       </c>
       <c r="G2" s="12">
-        <f>[18]Main!$O$8</f>
+        <f>[19]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[18]Main!$O$18</f>
+        <f>[19]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[18]Main!$O$3</f>
+        <f>[19]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[18]Main!$O$19</f>
+        <f>[19]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3402,19 +3512,19 @@
         <v>103</v>
       </c>
       <c r="G3" s="12">
-        <f>+[19]Main!$N$8</f>
+        <f>+[20]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[19]Main!$N$18</f>
+        <f>+[20]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[19]Main!$N$3</f>
+        <f>+[20]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[19]Main!$N$19</f>
+        <f>+[20]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3445,19 +3555,19 @@
         <v>108</v>
       </c>
       <c r="G4" s="12">
-        <f>[20]Main!$J$8</f>
+        <f>[21]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[20]Main!$J$18</f>
+        <f>[21]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[20]Main!$J$3</f>
+        <f>[21]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[20]Main!$J$19</f>
+        <f>[21]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2022Q4 DCF Update for ONSemiconductor (ON)
Pretty fairly valued.
Price target: $81.05
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C06148E-A635-4846-AA21-B2F95C871DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8683BA9E-23F9-4BEC-A417-5A77B7D723E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="1170" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="3210" yWindow="2940" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
     <externalReference r:id="rId26"/>
+    <externalReference r:id="rId27"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="133">
   <si>
     <t>Ticker</t>
   </si>
@@ -445,6 +446,12 @@
   </si>
   <si>
     <t>EBITDA/Sh</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>MRQ Release</t>
   </si>
 </sst>
 </file>
@@ -544,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -611,6 +618,8 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -999,34 +1008,54 @@
 <file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+        <row r="5">
+          <cell r="N5">
+            <v>185.65</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>99554.828000000009</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>95545.612738294119</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>188.40829140695323</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="29">
+          <cell r="J29">
+            <v>303.0739999999995</v>
+          </cell>
+          <cell r="K29">
+            <v>268.88500000000033</v>
+          </cell>
+          <cell r="L29">
+            <v>472.50999999999863</v>
+          </cell>
+          <cell r="M29">
+            <v>486.34199999999987</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1042,23 +1071,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1114,23 +1143,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1150,23 +1179,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1177,6 +1206,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1189,44 +1254,35 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="5">
-          <cell r="N5">
-            <v>185.65</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="N10">
-            <v>99554.828000000009</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="N13">
-            <v>95545.612738294119</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>188.40829140695323</v>
+        <row r="7">
+          <cell r="N7">
+            <v>76.28</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>34171.095999999998</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>35110.668973847663</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="N16">
+            <v>81.049559034736063</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="29">
-          <cell r="J29">
-            <v>303.0739999999995</v>
-          </cell>
-          <cell r="K29">
-            <v>268.88500000000033</v>
-          </cell>
-          <cell r="L29">
-            <v>472.50999999999863</v>
-          </cell>
-          <cell r="M29">
-            <v>486.34199999999987</v>
+          <cell r="X29">
+            <v>2922.8000000000011</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1781,11 +1837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W9" sqref="W9"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1793,16 +1849,16 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.5703125" style="19" customWidth="1"/>
     <col min="15" max="15" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1817,17 +1873,17 @@
       <c r="C1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>88</v>
@@ -1867,17 +1923,15 @@
       <c r="C2" s="4">
         <v>44775</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="22">
-        <v>44775</v>
       </c>
       <c r="H2" s="12">
         <f>[1]Main!$N$8</f>
@@ -1913,17 +1967,15 @@
       <c r="C3" s="4">
         <v>44772</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" s="22">
-        <v>44858</v>
       </c>
       <c r="H3" s="12">
         <f>[2]Main!$N$8</f>
@@ -1959,17 +2011,15 @@
       <c r="C4" s="4">
         <v>44773</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>51</v>
-      </c>
-      <c r="G4" s="22">
-        <v>44771</v>
       </c>
       <c r="H4" s="12">
         <f>[3]Main!$N$8</f>
@@ -2002,17 +2052,15 @@
       <c r="C5" s="4">
         <v>44773</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>58</v>
-      </c>
-      <c r="G5" s="22">
-        <v>44776</v>
       </c>
       <c r="H5" s="12">
         <f>[4]Main!$N$8</f>
@@ -2045,17 +2093,15 @@
       <c r="C6" s="4">
         <v>44773</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="30"/>
+      <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>62</v>
-      </c>
-      <c r="G6" s="22">
-        <v>44865</v>
       </c>
       <c r="H6" s="12">
         <f>[5]Main!$N$8</f>
@@ -2088,17 +2134,15 @@
       <c r="C7" s="4">
         <v>44774</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>63</v>
-      </c>
-      <c r="G7" s="22">
-        <v>44867</v>
       </c>
       <c r="H7" s="12">
         <f>[6]Main!$N$8</f>
@@ -2131,17 +2175,15 @@
       <c r="C8" s="4">
         <v>44774</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>66</v>
-      </c>
-      <c r="G8" s="22">
-        <v>44782</v>
       </c>
       <c r="H8" s="12">
         <f>[7]Main!$N$8</f>
@@ -2174,17 +2216,15 @@
       <c r="C9" s="4">
         <v>44774</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="30"/>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>79</v>
-      </c>
-      <c r="G9" s="22">
-        <v>44804</v>
       </c>
       <c r="H9" s="12">
         <f>[8]Main!$N$8</f>
@@ -2217,17 +2257,15 @@
       <c r="C10" s="4">
         <v>44775</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="30"/>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>69</v>
-      </c>
-      <c r="G10" s="22">
-        <v>44865</v>
       </c>
       <c r="H10" s="12">
         <f>[9]Main!$N$8</f>
@@ -2260,17 +2298,15 @@
       <c r="C11" s="4">
         <v>44775</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>73</v>
-      </c>
-      <c r="G11" s="22">
-        <v>44777</v>
       </c>
       <c r="H11" s="12">
         <f>[10]Main!$N$8</f>
@@ -2303,17 +2339,15 @@
       <c r="C12" s="4">
         <v>44775</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>78</v>
-      </c>
-      <c r="G12" s="22">
-        <v>44777</v>
       </c>
       <c r="H12" s="12">
         <f>[11]Main!$N$8</f>
@@ -2350,17 +2384,15 @@
       <c r="C13" s="4">
         <v>44778</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>100</v>
-      </c>
-      <c r="G13" s="22">
-        <v>44870</v>
       </c>
       <c r="H13" s="12">
         <f>[12]Main!$N$8</f>
@@ -2393,17 +2425,17 @@
       <c r="C14" s="4">
         <v>44973</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="30">
+        <v>44964</v>
+      </c>
+      <c r="E14" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="F14" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>120</v>
-      </c>
-      <c r="G14" s="22">
-        <v>45049</v>
       </c>
       <c r="H14" s="12">
         <f>[13]Main!$N$9</f>
@@ -2418,11 +2450,11 @@
         <v>642.59899999999948</v>
       </c>
       <c r="K14" s="29">
-        <f>J14/(I14/N14)</f>
+        <f t="shared" ref="K14:K20" si="1">J14/(I14/N14)</f>
         <v>2.519294627770305</v>
       </c>
       <c r="L14" s="28">
-        <f>H14/J14</f>
+        <f t="shared" ref="L14:L20" si="2">H14/J14</f>
         <v>65.181544400162522</v>
       </c>
       <c r="M14" s="19">
@@ -2448,17 +2480,17 @@
       <c r="C15" s="4">
         <v>44972</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="30">
+        <v>44916</v>
+      </c>
+      <c r="E15" t="s">
         <v>123</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="F15" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>119</v>
-      </c>
-      <c r="G15" s="22">
-        <v>45005</v>
       </c>
       <c r="H15" s="12">
         <f>[14]Main!$N$9</f>
@@ -2473,11 +2505,11 @@
         <v>-2103</v>
       </c>
       <c r="K15" s="29">
-        <f>J15/(I15/N15)</f>
+        <f t="shared" si="1"/>
         <v>-1.7809748892171344</v>
       </c>
       <c r="L15" s="28">
-        <f>H15/J15</f>
+        <f t="shared" si="2"/>
         <v>-20.909710933439491</v>
       </c>
       <c r="M15" s="19">
@@ -2503,17 +2535,17 @@
       <c r="C16" s="4">
         <v>44972</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="30">
+        <v>44873</v>
+      </c>
+      <c r="E16" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="F16" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>121</v>
-      </c>
-      <c r="G16" s="22">
-        <v>44985</v>
       </c>
       <c r="H16" s="12">
         <f>[15]Main!$N$9</f>
@@ -2527,11 +2559,11 @@
         <v>-724</v>
       </c>
       <c r="K16" s="29">
-        <f>J16/(I16/N16)</f>
+        <f t="shared" si="1"/>
         <v>-1.9811245892039655</v>
       </c>
       <c r="L16" s="28">
-        <f>H16/J16</f>
+        <f t="shared" si="2"/>
         <v>-26.90468009668508</v>
       </c>
       <c r="M16" s="19">
@@ -2557,17 +2589,17 @@
       <c r="C17" s="4">
         <v>44972</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="30">
+        <v>44867</v>
+      </c>
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="F17" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>122</v>
-      </c>
-      <c r="G17" s="22">
-        <v>44985</v>
       </c>
       <c r="H17" s="12">
         <f>[16]Main!$N$9</f>
@@ -2581,11 +2613,11 @@
         <v>2</v>
       </c>
       <c r="K17" s="29">
-        <f>J17/(I17/N17)</f>
+        <f t="shared" si="1"/>
         <v>3.7703836365350178E-2</v>
       </c>
       <c r="L17" s="28">
-        <f>H17/J17</f>
+        <f t="shared" si="2"/>
         <v>544.56130000000007</v>
       </c>
       <c r="M17" s="19">
@@ -2611,13 +2643,16 @@
       <c r="C18" s="4">
         <v>44979</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="30">
+        <v>44950</v>
+      </c>
+      <c r="E18" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="12">
@@ -2633,11 +2668,11 @@
         <v>11119</v>
       </c>
       <c r="K18" s="29">
-        <f>J18/(I18/N18)</f>
+        <f t="shared" si="1"/>
         <v>12.138646288209607</v>
       </c>
       <c r="L18" s="28">
-        <f>H18/J18</f>
+        <f t="shared" si="2"/>
         <v>14.035057109452291</v>
       </c>
       <c r="M18" s="19">
@@ -2663,46 +2698,104 @@
       <c r="C19" s="4">
         <v>44980</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="30">
+        <v>44972</v>
+      </c>
+      <c r="E19" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="12">
-        <f>[22]Main!$N$10</f>
+        <f>[18]Main!$N$10</f>
         <v>99554.828000000009</v>
       </c>
       <c r="I19" s="13">
-        <f>+[22]Main!$N$13</f>
+        <f>+[18]Main!$N$13</f>
         <v>95545.612738294119</v>
       </c>
       <c r="J19" s="13">
-        <f>SUM([22]Model!$J$29:$M$29)</f>
+        <f>SUM([18]Model!$J$29:$M$29)</f>
         <v>1530.8109999999983</v>
       </c>
       <c r="K19" s="29">
-        <f>J19/(I19/N19)</f>
+        <f t="shared" si="1"/>
         <v>3.0186366146079791</v>
       </c>
       <c r="L19" s="28">
-        <f>H19/J19</f>
+        <f t="shared" si="2"/>
         <v>65.034042739436885</v>
       </c>
       <c r="M19" s="19">
-        <f>+[22]Main!$N$5</f>
+        <f>+[18]Main!$N$5</f>
         <v>185.65</v>
       </c>
       <c r="N19" s="19">
-        <f>+[22]Main!$N$14</f>
+        <f>+[18]Main!$N$14</f>
         <v>188.40829140695323</v>
       </c>
       <c r="O19" s="14">
         <f>N19/M19</f>
         <v>1.0148574813194355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="4">
+        <v>44981</v>
+      </c>
+      <c r="D20" s="30">
+        <v>44963</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="12">
+        <f>+[23]Main!$N$12</f>
+        <v>34171.095999999998</v>
+      </c>
+      <c r="I20" s="13">
+        <f>+[23]Main!$N$15</f>
+        <v>35110.668973847663</v>
+      </c>
+      <c r="J20" s="13">
+        <f>+[23]Model!$X$29</f>
+        <v>2922.8000000000011</v>
+      </c>
+      <c r="K20" s="29">
+        <f t="shared" si="1"/>
+        <v>6.7469990766389687</v>
+      </c>
+      <c r="L20" s="28">
+        <f t="shared" si="2"/>
+        <v>11.691219378677975</v>
+      </c>
+      <c r="M20" s="19">
+        <f>+[23]Main!$N$7</f>
+        <v>76.28</v>
+      </c>
+      <c r="N20" s="19">
+        <f>+[23]Main!$N$16</f>
+        <v>81.049559034736063</v>
+      </c>
+      <c r="O20" s="14">
+        <f>N20/M20</f>
+        <v>1.0625269931140018</v>
       </c>
     </row>
   </sheetData>
@@ -2719,27 +2812,28 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{73328F8B-1F94-4A8A-9A78-403E164E8CF5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{9DBC66B9-2FF1-4977-B2DF-8C41D4A7A6D1}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{13EDAF3C-5721-4D75-9703-2DB05A32F554}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{1F57513D-24D3-4658-8F68-AF40A09EFC74}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{7760A594-AEAF-4B58-817B-4761F7B99113}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{F26D788E-1A4C-438C-9388-1DE3F435DDD3}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{C5B7B287-A56A-4BF1-A85C-5D722595DDC9}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{608B7647-1B08-4C9F-9F67-8EE648DE91F4}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{EC971D85-AE4D-4BAC-8F79-E09E5BB1E48F}"/>
-    <hyperlink ref="E10" r:id="rId10" xr:uid="{3F8536C2-23A7-4161-812E-20365E1D9978}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{EADEAE13-3EB5-4DD8-A227-962C1710AB1F}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{8891FA92-2D91-4B39-8F9A-15A7A99C6B0E}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{B17BAEAB-F391-4432-AAF4-5E33835BE8BD}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{C1F4114B-46BB-4059-A5BE-C706C0D64BF9}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{6B733B71-6254-4B4B-A709-845BAA354A79}"/>
-    <hyperlink ref="E17" r:id="rId16" xr:uid="{8C7CEC3F-9A88-4BF1-8E7D-6185C3B6C9AF}"/>
-    <hyperlink ref="E18" r:id="rId17" xr:uid="{0B716ECA-DE4E-45F0-86A2-02472C2F8EAB}"/>
-    <hyperlink ref="E19" r:id="rId18" xr:uid="{9712A0F2-E276-4023-8E1C-20FFFF3D79AF}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{73328F8B-1F94-4A8A-9A78-403E164E8CF5}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{9DBC66B9-2FF1-4977-B2DF-8C41D4A7A6D1}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{13EDAF3C-5721-4D75-9703-2DB05A32F554}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{1F57513D-24D3-4658-8F68-AF40A09EFC74}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{7760A594-AEAF-4B58-817B-4761F7B99113}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{F26D788E-1A4C-438C-9388-1DE3F435DDD3}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{C5B7B287-A56A-4BF1-A85C-5D722595DDC9}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{608B7647-1B08-4C9F-9F67-8EE648DE91F4}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{EC971D85-AE4D-4BAC-8F79-E09E5BB1E48F}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{3F8536C2-23A7-4161-812E-20365E1D9978}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{EADEAE13-3EB5-4DD8-A227-962C1710AB1F}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{8891FA92-2D91-4B39-8F9A-15A7A99C6B0E}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{B17BAEAB-F391-4432-AAF4-5E33835BE8BD}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{C1F4114B-46BB-4059-A5BE-C706C0D64BF9}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{6B733B71-6254-4B4B-A709-845BAA354A79}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{8C7CEC3F-9A88-4BF1-8E7D-6185C3B6C9AF}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{0B716ECA-DE4E-45F0-86A2-02472C2F8EAB}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{9712A0F2-E276-4023-8E1C-20FFFF3D79AF}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{D51FB28B-25B5-4085-89BA-B30029424F9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2748,7 +2842,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,7 +3101,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,19 +3271,19 @@
         <v>33</v>
       </c>
       <c r="G6" s="12">
-        <f>+[18]Main!$J$8</f>
+        <f>+[19]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[18]Main!$J$18</f>
+        <f>+[19]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[18]Main!$J$3</f>
+        <f>+[19]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[18]Main!$J$19</f>
+        <f>+[19]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3472,19 +3566,19 @@
         <v>97</v>
       </c>
       <c r="G2" s="12">
-        <f>[19]Main!$O$8</f>
+        <f>[20]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[19]Main!$O$18</f>
+        <f>[20]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[19]Main!$O$3</f>
+        <f>[20]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[19]Main!$O$19</f>
+        <f>[20]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3512,19 +3606,19 @@
         <v>103</v>
       </c>
       <c r="G3" s="12">
-        <f>+[20]Main!$N$8</f>
+        <f>+[21]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[20]Main!$N$18</f>
+        <f>+[21]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[20]Main!$N$3</f>
+        <f>+[21]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[20]Main!$N$19</f>
+        <f>+[21]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3555,19 +3649,19 @@
         <v>108</v>
       </c>
       <c r="G4" s="12">
-        <f>[21]Main!$J$8</f>
+        <f>[22]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[21]Main!$J$18</f>
+        <f>[22]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[21]Main!$J$3</f>
+        <f>[22]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[21]Main!$J$19</f>
+        <f>[22]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2023Q3 DCF Update for Microchip Technology (MCHP)
Pretty fairly valued.
Price target: $89.94
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8683BA9E-23F9-4BEC-A417-5A77B7D723E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8464BA7-56C7-406F-829F-1DF261461725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2940" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="16080" yWindow="4710" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,7 @@
     <externalReference r:id="rId25"/>
     <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
+    <externalReference r:id="rId28"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="137">
   <si>
     <t>Ticker</t>
   </si>
@@ -452,6 +453,18 @@
   </si>
   <si>
     <t>MRQ Release</t>
+  </si>
+  <si>
+    <t>23Q3</t>
+  </si>
+  <si>
+    <t>MCHP</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MkCap</t>
   </si>
 </sst>
 </file>
@@ -618,8 +631,10 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -800,6 +815,11 @@
             <v>75.75</v>
           </cell>
         </row>
+        <row r="6">
+          <cell r="N6">
+            <v>19321.628250000002</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="N9">
             <v>41885.595249999998</v>
@@ -823,7 +843,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -847,6 +867,11 @@
             <v>12.19</v>
           </cell>
         </row>
+        <row r="6">
+          <cell r="N6">
+            <v>14394.122093023256</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="N9">
             <v>43973.122093023252</v>
@@ -870,7 +895,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -894,6 +919,11 @@
             <v>18.11</v>
           </cell>
         </row>
+        <row r="6">
+          <cell r="N6">
+            <v>6618.2813900000001</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="N9">
             <v>19478.988389999999</v>
@@ -910,8 +940,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -935,6 +965,11 @@
             <v>11.68</v>
           </cell>
         </row>
+        <row r="6">
+          <cell r="N6">
+            <v>619.56560000000002</v>
+          </cell>
+        </row>
         <row r="9">
           <cell r="N9">
             <v>1089.1226000000001</v>
@@ -951,8 +986,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -974,6 +1009,11 @@
         <row r="5">
           <cell r="N5">
             <v>169.8</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="N7">
+            <v>155536.80000000002</v>
           </cell>
         </row>
         <row r="10">
@@ -1023,6 +1063,11 @@
             <v>185.65</v>
           </cell>
         </row>
+        <row r="7">
+          <cell r="N7">
+            <v>94146.828000000009</v>
+          </cell>
+        </row>
         <row r="10">
           <cell r="N10">
             <v>99554.828000000009</v>
@@ -1055,7 +1100,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1064,34 +1109,50 @@
 <file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+        <row r="7">
+          <cell r="N7">
+            <v>76.28</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="N9">
+            <v>33044.495999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>34171.095999999998</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>35110.668973847663</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="N16">
+            <v>81.049559034736063</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="29">
+          <cell r="X29">
+            <v>2922.8000000000011</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1143,23 +1204,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1179,23 +1240,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1215,23 +1276,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1242,6 +1303,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1254,35 +1351,49 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="7">
-          <cell r="N7">
-            <v>76.28</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="N12">
-            <v>34171.095999999998</v>
+        <row r="6">
+          <cell r="N6">
+            <v>79.680000000000007</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>43760.256000000008</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>50060.056000000004</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>49396.022818172591</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>35110.668973847663</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="N16">
-            <v>81.049559034736063</v>
+            <v>89.941774978464281</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="29">
-          <cell r="X29">
-            <v>2922.8000000000011</v>
+        <row r="28">
+          <cell r="F28">
+            <v>854.99999999999932</v>
+          </cell>
+          <cell r="G28">
+            <v>964.69999999999982</v>
+          </cell>
+          <cell r="H28">
+            <v>1011.1999999999999</v>
+          </cell>
+          <cell r="I28">
+            <v>1059.7999999999997</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1837,11 +1948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1849,21 +1960,22 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.5703125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" style="19" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1889,31 +2001,34 @@
         <v>88</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1937,27 +2052,27 @@
         <f>[1]Main!$N$8</f>
         <v>5262.9334767642013</v>
       </c>
-      <c r="I2" s="13">
+      <c r="J2" s="13">
         <f>[1]Main!$N$19</f>
         <v>22198.677928000903</v>
       </c>
-      <c r="M2" s="19">
+      <c r="N2" s="19">
         <f>[1]Main!$N$3</f>
         <v>107</v>
       </c>
-      <c r="N2" s="19">
+      <c r="O2" s="19">
         <f>[1]Main!$N$20</f>
         <v>506.49669636225735</v>
       </c>
-      <c r="O2" s="14">
-        <f>N2/M2</f>
+      <c r="P2" s="14">
+        <f>O2/N2</f>
         <v>4.733613984693994</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -1981,27 +2096,27 @@
         <f>[2]Main!$N$8</f>
         <v>2219.4089300000001</v>
       </c>
-      <c r="I3" s="13">
+      <c r="J3" s="13">
         <f>[2]Main!$N$18</f>
         <v>11759.15586027935</v>
       </c>
-      <c r="M3" s="19">
+      <c r="N3" s="19">
         <f>[2]Main!$N$3</f>
         <v>138.47</v>
       </c>
-      <c r="N3" s="19">
+      <c r="O3" s="19">
         <f>[2]Main!$N$19</f>
         <v>605.54899120857669</v>
       </c>
-      <c r="O3" s="14">
-        <f>N3/M3</f>
+      <c r="P3" s="14">
+        <f>O3/N3</f>
         <v>4.3731421333760139</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -2025,24 +2140,24 @@
         <f>[3]Main!$N$8</f>
         <v>7062.3840000000009</v>
       </c>
-      <c r="I4" s="13">
+      <c r="J4" s="13">
         <f>[3]Main!$N$18</f>
         <v>8817.3705876180775</v>
       </c>
-      <c r="M4" s="19">
+      <c r="N4" s="19">
         <f>[3]Main!$N$3</f>
         <v>35.31</v>
       </c>
-      <c r="N4" s="19">
+      <c r="O4" s="19">
         <f>[3]Main!$N$19</f>
         <v>52.989005935204794</v>
       </c>
-      <c r="O4" s="14">
-        <f t="shared" ref="O4:O17" si="0">N4/M4</f>
+      <c r="P4" s="14">
+        <f t="shared" ref="P4:P17" si="0">O4/N4</f>
         <v>1.5006798622261339</v>
       </c>
     </row>
-    <row r="5" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -2066,24 +2181,24 @@
         <f>[4]Main!$N$8</f>
         <v>3670.81792</v>
       </c>
-      <c r="I5" s="13">
+      <c r="J5" s="13">
         <f>[4]Main!$N$19</f>
         <v>2996.7820265448186</v>
       </c>
-      <c r="M5" s="19">
+      <c r="N5" s="19">
         <f>[4]Main!$N$3</f>
         <v>64.72</v>
       </c>
-      <c r="N5" s="19">
+      <c r="O5" s="19">
         <f>[4]Main!$N$20</f>
         <v>66.876035494517382</v>
       </c>
-      <c r="O5" s="14">
+      <c r="P5" s="14">
         <f t="shared" si="0"/>
         <v>1.0333132801995888</v>
       </c>
     </row>
-    <row r="6" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2107,24 +2222,24 @@
         <f>[5]Main!$N$8</f>
         <v>1029.8218324607337</v>
       </c>
-      <c r="I6" s="13">
+      <c r="J6" s="13">
         <f>[5]Main!$N$18</f>
         <v>4076.5725319753483</v>
       </c>
-      <c r="M6" s="19">
+      <c r="N6" s="19">
         <f>[5]Main!$N$3</f>
         <v>87</v>
       </c>
-      <c r="N6" s="19">
+      <c r="O6" s="19">
         <f>[5]Main!$N$19</f>
         <v>436.69397285882815</v>
       </c>
-      <c r="O6" s="14">
+      <c r="P6" s="14">
         <f t="shared" si="0"/>
         <v>5.0194709524003231</v>
       </c>
     </row>
-    <row r="7" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -2148,24 +2263,24 @@
         <f>[6]Main!$N$8</f>
         <v>15906.644</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="13">
         <f>[6]Main!$N$18</f>
         <v>50207.036438406729</v>
       </c>
-      <c r="M7" s="19">
+      <c r="N7" s="19">
         <f>[6]Main!$N$3</f>
         <v>73.459999999999994</v>
       </c>
-      <c r="N7" s="19">
+      <c r="O7" s="19">
         <f>[6]Main!$N$19</f>
         <v>294.64223261975781</v>
       </c>
-      <c r="O7" s="14">
+      <c r="P7" s="14">
         <f t="shared" si="0"/>
         <v>4.0109206727437767</v>
       </c>
     </row>
-    <row r="8" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -2189,24 +2304,24 @@
         <f>[7]Main!$N$8</f>
         <v>5265.84</v>
       </c>
-      <c r="I8" s="13">
+      <c r="J8" s="13">
         <f>[7]Main!$N$18</f>
         <v>12229.883434318077</v>
       </c>
-      <c r="M8" s="19">
+      <c r="N8" s="19">
         <f>[7]Main!$N$3</f>
         <v>64.44</v>
       </c>
-      <c r="N8" s="19">
+      <c r="O8" s="19">
         <f>[7]Main!$N$19</f>
         <v>142.2079469106753</v>
       </c>
-      <c r="O8" s="14">
+      <c r="P8" s="14">
         <f t="shared" si="0"/>
         <v>2.2068272332507033</v>
       </c>
     </row>
-    <row r="9" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -2230,24 +2345,24 @@
         <f>[8]Main!$N$8</f>
         <v>877.07125999999994</v>
       </c>
-      <c r="I9" s="13">
+      <c r="J9" s="13">
         <f>[8]Main!$N$18</f>
         <v>1643.4101590621442</v>
       </c>
-      <c r="M9" s="19">
+      <c r="N9" s="19">
         <f>[8]Main!$N$3</f>
         <v>25.18</v>
       </c>
-      <c r="N9" s="19">
+      <c r="O9" s="19">
         <f>[8]Main!$N$19</f>
         <v>49.564500982059428</v>
       </c>
-      <c r="O9" s="14">
+      <c r="P9" s="14">
         <f t="shared" si="0"/>
         <v>1.9684075052446159</v>
       </c>
     </row>
-    <row r="10" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -2271,24 +2386,24 @@
         <f>[9]Main!$N$8</f>
         <v>6531.1078800000005</v>
       </c>
-      <c r="I10" s="13">
+      <c r="J10" s="13">
         <f>[9]Main!$N$18</f>
         <v>8831.5667844635373</v>
       </c>
-      <c r="M10" s="19">
+      <c r="N10" s="19">
         <f>[9]Main!$N$3</f>
         <v>260.32</v>
       </c>
-      <c r="N10" s="19">
+      <c r="O10" s="19">
         <f>[9]Main!$N$19</f>
         <v>357.06180902658434</v>
       </c>
-      <c r="O10" s="14">
+      <c r="P10" s="14">
         <f t="shared" si="0"/>
         <v>1.3716264944168115</v>
       </c>
     </row>
-    <row r="11" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2312,24 +2427,24 @@
         <f>[10]Main!$N$8</f>
         <v>5961.5730000000003</v>
       </c>
-      <c r="I11" s="13">
+      <c r="J11" s="13">
         <f>[10]Main!$N$18</f>
         <v>6053.073284927159</v>
       </c>
-      <c r="M11" s="19">
+      <c r="N11" s="19">
         <f>[10]Main!$N$3</f>
         <v>60.73</v>
       </c>
-      <c r="N11" s="19">
+      <c r="O11" s="19">
         <f>[10]Main!$N$19</f>
         <v>86.349119613796859</v>
       </c>
-      <c r="O11" s="14">
-        <f>N11/M11</f>
+      <c r="P11" s="14">
+        <f>O11/N11</f>
         <v>1.4218527846829716</v>
       </c>
     </row>
-    <row r="12" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2353,28 +2468,28 @@
         <f>[11]Main!$N$8</f>
         <v>3705.70046</v>
       </c>
-      <c r="I12" s="13">
+      <c r="J12" s="13">
         <f>[11]Main!$N$18</f>
         <v>2666.8844433216959</v>
       </c>
-      <c r="M12" s="19">
+      <c r="N12" s="19">
         <f>[11]Main!$N$3</f>
         <v>20.86</v>
       </c>
-      <c r="N12" s="19">
+      <c r="O12" s="19">
         <f>[11]Main!$N$19</f>
         <v>17.243419112262924</v>
       </c>
-      <c r="O12" s="14">
+      <c r="P12" s="14">
         <f t="shared" si="0"/>
         <v>0.82662603606246043</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>89</v>
       </c>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -2398,24 +2513,24 @@
         <f>[12]Main!$N$8</f>
         <v>31004.120000000003</v>
       </c>
-      <c r="I13" s="13">
+      <c r="J13" s="13">
         <f>[12]Main!$N$18</f>
         <v>59674.776053903901</v>
       </c>
-      <c r="M13" s="19">
+      <c r="N13" s="19">
         <f>[12]Main!$N$3</f>
         <v>76.150000000000006</v>
       </c>
-      <c r="N13" s="19">
+      <c r="O13" s="19">
         <f>[12]Main!$N$19</f>
         <v>170.11053607156185</v>
       </c>
-      <c r="O13" s="14">
+      <c r="P13" s="14">
         <f t="shared" si="0"/>
         <v>2.2338875386941806</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -2441,36 +2556,40 @@
         <f>[13]Main!$N$9</f>
         <v>41885.595249999998</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="31">
+        <f>+[13]Main!$N$6</f>
+        <v>19321.628250000002</v>
+      </c>
+      <c r="J14" s="13">
         <f>[13]Main!$N$12</f>
         <v>17718.474111348907</v>
       </c>
-      <c r="J14" s="13">
+      <c r="K14" s="13">
         <f>+[13]Model!$AA$27</f>
         <v>642.59899999999948</v>
       </c>
-      <c r="K14" s="29">
-        <f t="shared" ref="K14:K20" si="1">J14/(I14/N14)</f>
+      <c r="L14" s="29">
+        <f t="shared" ref="L14:L21" si="1">K14/(J14/O14)</f>
         <v>2.519294627770305</v>
       </c>
-      <c r="L14" s="28">
-        <f t="shared" ref="L14:L20" si="2">H14/J14</f>
+      <c r="M14" s="28">
+        <f t="shared" ref="M14:M21" si="2">H14/K14</f>
         <v>65.181544400162522</v>
       </c>
-      <c r="M14" s="19">
+      <c r="N14" s="19">
         <f>[13]Main!$N$4</f>
         <v>75.75</v>
       </c>
-      <c r="N14" s="19">
+      <c r="O14" s="19">
         <f>[13]Main!$N$13</f>
         <v>69.464871001991241</v>
       </c>
-      <c r="O14" s="14">
+      <c r="P14" s="14">
         <f t="shared" si="0"/>
         <v>0.91702800002628704</v>
       </c>
     </row>
-    <row r="15" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2496,36 +2615,40 @@
         <f>[14]Main!$N$9</f>
         <v>43973.122093023252</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="31">
+        <f>+[14]Main!$N$6</f>
+        <v>14394.122093023256</v>
+      </c>
+      <c r="J15" s="13">
         <f>[14]Main!$N$12</f>
         <v>18848.439289507303</v>
       </c>
-      <c r="J15" s="13">
+      <c r="K15" s="13">
         <f>+[14]Model!$Z$27</f>
         <v>-2103</v>
       </c>
-      <c r="K15" s="29">
+      <c r="L15" s="29">
         <f t="shared" si="1"/>
         <v>-1.7809748892171344</v>
       </c>
-      <c r="L15" s="28">
+      <c r="M15" s="28">
         <f t="shared" si="2"/>
         <v>-20.909710933439491</v>
       </c>
-      <c r="M15" s="19">
+      <c r="N15" s="19">
         <f>[14]Main!$N$4</f>
         <v>12.19</v>
       </c>
-      <c r="N15" s="19">
+      <c r="O15" s="19">
         <f>[14]Main!$N$13</f>
         <v>15.962243022133215</v>
       </c>
-      <c r="O15" s="14">
+      <c r="P15" s="14">
         <f t="shared" si="0"/>
         <v>1.3094538984522737</v>
       </c>
     </row>
-    <row r="16" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -2551,35 +2674,39 @@
         <f>[15]Main!$N$9</f>
         <v>19478.988389999999</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="31">
+        <f>+[15]Main!$N$6</f>
+        <v>6618.2813900000001</v>
+      </c>
+      <c r="J16" s="13">
         <f>[15]Main!$N$12</f>
         <v>9576.3280554549001</v>
       </c>
-      <c r="J16" s="13">
+      <c r="K16" s="13">
         <v>-724</v>
       </c>
-      <c r="K16" s="29">
+      <c r="L16" s="29">
         <f t="shared" si="1"/>
         <v>-1.9811245892039655</v>
       </c>
-      <c r="L16" s="28">
+      <c r="M16" s="28">
         <f t="shared" si="2"/>
         <v>-26.90468009668508</v>
       </c>
-      <c r="M16" s="19">
+      <c r="N16" s="19">
         <f>[15]Main!$N$4</f>
         <v>18.11</v>
       </c>
-      <c r="N16" s="19">
+      <c r="O16" s="19">
         <f>[15]Main!$N$13</f>
         <v>26.204280365946822</v>
       </c>
-      <c r="O16" s="14">
+      <c r="P16" s="14">
         <f t="shared" si="0"/>
         <v>1.4469508760876213</v>
       </c>
     </row>
-    <row r="17" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2605,35 +2732,39 @@
         <f>[16]Main!$N$9</f>
         <v>1089.1226000000001</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="31">
+        <f>+[16]Main!$N$6</f>
+        <v>619.56560000000002</v>
+      </c>
+      <c r="J17" s="13">
         <f>[16]Main!$N$12</f>
         <v>473.84250172820322</v>
       </c>
-      <c r="J17" s="13">
+      <c r="K17" s="13">
         <v>2</v>
       </c>
-      <c r="K17" s="29">
+      <c r="L17" s="29">
         <f t="shared" si="1"/>
         <v>3.7703836365350178E-2</v>
       </c>
-      <c r="L17" s="28">
+      <c r="M17" s="28">
         <f t="shared" si="2"/>
         <v>544.56130000000007</v>
       </c>
-      <c r="M17" s="19">
+      <c r="N17" s="19">
         <f>[16]Main!$N$4</f>
         <v>11.68</v>
       </c>
-      <c r="N17" s="19">
+      <c r="O17" s="19">
         <f>[16]Main!$N$13</f>
         <v>8.932840074054166</v>
       </c>
-      <c r="O17" s="14">
+      <c r="P17" s="14">
         <f t="shared" si="0"/>
         <v>0.76479795154573338</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -2659,36 +2790,40 @@
         <f>[17]Main!$N$10</f>
         <v>156055.80000000002</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="31">
+        <f>+[17]Main!$N$7</f>
+        <v>155536.80000000002</v>
+      </c>
+      <c r="J18" s="13">
         <f>[17]Main!$N$12</f>
         <v>134489.60313830531</v>
       </c>
-      <c r="J18" s="13">
+      <c r="K18" s="13">
         <f>[17]Model!$X$28</f>
         <v>11119</v>
       </c>
-      <c r="K18" s="29">
+      <c r="L18" s="29">
         <f t="shared" si="1"/>
         <v>12.138646288209607</v>
       </c>
-      <c r="L18" s="28">
+      <c r="M18" s="28">
         <f t="shared" si="2"/>
         <v>14.035057109452291</v>
       </c>
-      <c r="M18" s="19">
+      <c r="N18" s="19">
         <f>[17]Main!$N$5</f>
         <v>169.8</v>
       </c>
-      <c r="N18" s="19">
+      <c r="O18" s="19">
         <f>[17]Main!$N$13</f>
         <v>146.82271084967829</v>
       </c>
-      <c r="O18" s="14">
-        <f>N18/M18</f>
+      <c r="P18" s="14">
+        <f>O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -2714,36 +2849,40 @@
         <f>[18]Main!$N$10</f>
         <v>99554.828000000009</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="31">
+        <f>+[18]Main!$N$7</f>
+        <v>94146.828000000009</v>
+      </c>
+      <c r="J19" s="13">
         <f>+[18]Main!$N$13</f>
         <v>95545.612738294119</v>
       </c>
-      <c r="J19" s="13">
+      <c r="K19" s="13">
         <f>SUM([18]Model!$J$29:$M$29)</f>
         <v>1530.8109999999983</v>
       </c>
-      <c r="K19" s="29">
+      <c r="L19" s="29">
         <f t="shared" si="1"/>
         <v>3.0186366146079791</v>
       </c>
-      <c r="L19" s="28">
+      <c r="M19" s="28">
         <f t="shared" si="2"/>
         <v>65.034042739436885</v>
       </c>
-      <c r="M19" s="19">
+      <c r="N19" s="19">
         <f>+[18]Main!$N$5</f>
         <v>185.65</v>
       </c>
-      <c r="N19" s="19">
+      <c r="O19" s="19">
         <f>+[18]Main!$N$14</f>
         <v>188.40829140695323</v>
       </c>
-      <c r="O19" s="14">
-        <f>N19/M19</f>
+      <c r="P19" s="14">
+        <f>O19/N19</f>
         <v>1.0148574813194355</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -2766,40 +2905,103 @@
         <v>131</v>
       </c>
       <c r="H20" s="12">
-        <f>+[23]Main!$N$12</f>
+        <f>+[19]Main!$N$12</f>
         <v>34171.095999999998</v>
       </c>
-      <c r="I20" s="13">
-        <f>+[23]Main!$N$15</f>
+      <c r="I20" s="31">
+        <f>+[19]Main!$N$9</f>
+        <v>33044.495999999999</v>
+      </c>
+      <c r="J20" s="13">
+        <f>+[19]Main!$N$15</f>
         <v>35110.668973847663</v>
       </c>
-      <c r="J20" s="13">
-        <f>+[23]Model!$X$29</f>
+      <c r="K20" s="13">
+        <f>+[19]Model!$X$29</f>
         <v>2922.8000000000011</v>
       </c>
-      <c r="K20" s="29">
+      <c r="L20" s="29">
         <f t="shared" si="1"/>
         <v>6.7469990766389687</v>
       </c>
-      <c r="L20" s="28">
+      <c r="M20" s="28">
         <f t="shared" si="2"/>
         <v>11.691219378677975</v>
       </c>
-      <c r="M20" s="19">
-        <f>+[23]Main!$N$7</f>
+      <c r="N20" s="19">
+        <f>+[19]Main!$N$7</f>
         <v>76.28</v>
       </c>
-      <c r="N20" s="19">
-        <f>+[23]Main!$N$16</f>
+      <c r="O20" s="19">
+        <f>+[19]Main!$N$16</f>
         <v>81.049559034736063</v>
       </c>
-      <c r="O20" s="14">
-        <f>N20/M20</f>
+      <c r="P20" s="14">
+        <f>O20/N20</f>
         <v>1.0625269931140018</v>
       </c>
     </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="4">
+        <v>44982</v>
+      </c>
+      <c r="D21" s="30">
+        <v>44959</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="12">
+        <f>+[24]Main!$N$11</f>
+        <v>50060.056000000004</v>
+      </c>
+      <c r="I21" s="31">
+        <f>+[24]Main!$N$8</f>
+        <v>43760.256000000008</v>
+      </c>
+      <c r="J21" s="13">
+        <f>+[24]Main!$N$14</f>
+        <v>49396.022818172591</v>
+      </c>
+      <c r="K21" s="13">
+        <f>+SUM([24]Model!$F$28:$I$28)</f>
+        <v>3890.6999999999989</v>
+      </c>
+      <c r="L21" s="29">
+        <f t="shared" si="1"/>
+        <v>7.0843044428259256</v>
+      </c>
+      <c r="M21" s="28">
+        <f t="shared" si="2"/>
+        <v>12.866593672089859</v>
+      </c>
+      <c r="N21" s="19">
+        <f>+[24]Main!$N$6</f>
+        <v>79.680000000000007</v>
+      </c>
+      <c r="O21" s="19">
+        <f>+[24]Main!$N$15</f>
+        <v>89.941774978464281</v>
+      </c>
+      <c r="P21" s="14">
+        <f>O21/N21</f>
+        <v>1.1287873365771119</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O1:O1048576">
+  <conditionalFormatting sqref="P1:P1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2831,9 +3033,10 @@
     <hyperlink ref="F18" r:id="rId17" xr:uid="{0B716ECA-DE4E-45F0-86A2-02472C2F8EAB}"/>
     <hyperlink ref="F19" r:id="rId18" xr:uid="{9712A0F2-E276-4023-8E1C-20FFFF3D79AF}"/>
     <hyperlink ref="F20" r:id="rId19" xr:uid="{D51FB28B-25B5-4085-89BA-B30029424F9C}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{A5AEC059-A102-4726-A849-58E7EC9248D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -2842,7 +3045,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,19 +3474,19 @@
         <v>33</v>
       </c>
       <c r="G6" s="12">
-        <f>+[19]Main!$J$8</f>
+        <f>+[20]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[19]Main!$J$18</f>
+        <f>+[20]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[19]Main!$J$3</f>
+        <f>+[20]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[19]Main!$J$19</f>
+        <f>+[20]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3566,19 +3769,19 @@
         <v>97</v>
       </c>
       <c r="G2" s="12">
-        <f>[20]Main!$O$8</f>
+        <f>[21]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[20]Main!$O$18</f>
+        <f>[21]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[20]Main!$O$3</f>
+        <f>[21]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[20]Main!$O$19</f>
+        <f>[21]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3606,19 +3809,19 @@
         <v>103</v>
       </c>
       <c r="G3" s="12">
-        <f>+[21]Main!$N$8</f>
+        <f>+[22]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[21]Main!$N$18</f>
+        <f>+[22]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[21]Main!$N$3</f>
+        <f>+[22]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[21]Main!$N$19</f>
+        <f>+[22]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3649,19 +3852,19 @@
         <v>108</v>
       </c>
       <c r="G4" s="12">
-        <f>[22]Main!$J$8</f>
+        <f>[23]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[22]Main!$J$18</f>
+        <f>[23]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[22]Main!$J$3</f>
+        <f>[23]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[22]Main!$J$19</f>
+        <f>[23]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2023Q3 DCF for Semtech Corp (SMTC)
Pretty fairly valued. Their acquisition could screw them, too risky for me.
Price target: $34.09
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8464BA7-56C7-406F-829F-1DF261461725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C228F9-BE6B-495D-8349-03C6DDDA3E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="4710" windowWidth="32700" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="16545" yWindow="6030" windowWidth="27045" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,7 @@
     <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="144">
   <si>
     <t>Ticker</t>
   </si>
@@ -465,6 +466,27 @@
   </si>
   <si>
     <t>MkCap</t>
+  </si>
+  <si>
+    <t>SMTC</t>
+  </si>
+  <si>
+    <t>Semtech Corp</t>
+  </si>
+  <si>
+    <t>20% fab outsourced, looking to reduce</t>
+  </si>
+  <si>
+    <t>60% fab outsourced, looking to reduce</t>
+  </si>
+  <si>
+    <t>43% fab outsourced, looking to increase</t>
+  </si>
+  <si>
+    <t>&gt;50% fab outsourced, looking to maintain/increase</t>
+  </si>
+  <si>
+    <t>100% fab outsourced, is the 2023Q3 acquisition bullish?</t>
   </si>
 </sst>
 </file>
@@ -564,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -632,9 +654,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -843,7 +862,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -895,7 +914,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -940,8 +959,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -986,8 +1005,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1039,7 +1058,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1197,34 +1216,59 @@
 <file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="6">
+          <cell r="N6">
+            <v>79.680000000000007</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>43760.256000000008</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>50060.056000000004</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>49396.022818172591</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>89.941774978464281</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="F28">
+            <v>854.99999999999932</v>
+          </cell>
+          <cell r="G28">
+            <v>964.69999999999982</v>
+          </cell>
+          <cell r="H28">
+            <v>1011.1999999999999</v>
+          </cell>
+          <cell r="I28">
+            <v>1059.7999999999997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1240,23 +1284,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1276,23 +1320,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1312,23 +1356,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1339,6 +1383,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1353,43 +1433,43 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="N6">
-            <v>79.680000000000007</v>
+            <v>30.52</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>43760.256000000008</v>
+            <v>1946.07728</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>50060.056000000004</v>
+            <v>1828.46028</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>49396.022818172591</v>
+            <v>2173.7463596759726</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>89.941774978464281</v>
+            <v>34.090495572360147</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="28">
           <cell r="F28">
-            <v>854.99999999999932</v>
+            <v>52.289999999999864</v>
           </cell>
           <cell r="G28">
-            <v>964.69999999999982</v>
+            <v>55.844000000000015</v>
           </cell>
           <cell r="H28">
-            <v>1011.1999999999999</v>
+            <v>72.525999999999996</v>
           </cell>
           <cell r="I28">
-            <v>1059.7999999999997</v>
+            <v>45.867000000000004</v>
           </cell>
         </row>
       </sheetData>
@@ -1948,11 +2028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1965,9 +2045,9 @@
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="31" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="13" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5703125" style="19" customWidth="1"/>
@@ -2556,7 +2636,7 @@
         <f>[13]Main!$N$9</f>
         <v>41885.595249999998</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="13">
         <f>+[13]Main!$N$6</f>
         <v>19321.628250000002</v>
       </c>
@@ -2569,11 +2649,11 @@
         <v>642.59899999999948</v>
       </c>
       <c r="L14" s="29">
-        <f t="shared" ref="L14:L21" si="1">K14/(J14/O14)</f>
+        <f t="shared" ref="L14:L22" si="1">K14/(J14/O14)</f>
         <v>2.519294627770305</v>
       </c>
       <c r="M14" s="28">
-        <f t="shared" ref="M14:M21" si="2">H14/K14</f>
+        <f t="shared" ref="M14:M22" si="2">H14/K14</f>
         <v>65.181544400162522</v>
       </c>
       <c r="N14" s="19">
@@ -2615,7 +2695,7 @@
         <f>[14]Main!$N$9</f>
         <v>43973.122093023252</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="13">
         <f>+[14]Main!$N$6</f>
         <v>14394.122093023256</v>
       </c>
@@ -2674,7 +2754,7 @@
         <f>[15]Main!$N$9</f>
         <v>19478.988389999999</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="13">
         <f>+[15]Main!$N$6</f>
         <v>6618.2813900000001</v>
       </c>
@@ -2706,7 +2786,7 @@
         <v>1.4469508760876213</v>
       </c>
     </row>
-    <row r="17" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2732,7 +2812,7 @@
         <f>[16]Main!$N$9</f>
         <v>1089.1226000000001</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="13">
         <f>+[16]Main!$N$6</f>
         <v>619.56560000000002</v>
       </c>
@@ -2764,7 +2844,7 @@
         <v>0.76479795154573338</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -2790,7 +2870,7 @@
         <f>[17]Main!$N$10</f>
         <v>156055.80000000002</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="13">
         <f>+[17]Main!$N$7</f>
         <v>155536.80000000002</v>
       </c>
@@ -2822,8 +2902,11 @@
         <f>O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -2849,7 +2932,7 @@
         <f>[18]Main!$N$10</f>
         <v>99554.828000000009</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="13">
         <f>+[18]Main!$N$7</f>
         <v>94146.828000000009</v>
       </c>
@@ -2881,8 +2964,11 @@
         <f>O19/N19</f>
         <v>1.0148574813194355</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -2908,7 +2994,7 @@
         <f>+[19]Main!$N$12</f>
         <v>34171.095999999998</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="13">
         <f>+[19]Main!$N$9</f>
         <v>33044.495999999999</v>
       </c>
@@ -2940,8 +3026,11 @@
         <f>O20/N20</f>
         <v>1.0625269931140018</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -2964,19 +3053,19 @@
         <v>135</v>
       </c>
       <c r="H21" s="12">
-        <f>+[24]Main!$N$11</f>
+        <f>+[20]Main!$N$11</f>
         <v>50060.056000000004</v>
       </c>
-      <c r="I21" s="31">
-        <f>+[24]Main!$N$8</f>
+      <c r="I21" s="13">
+        <f>+[20]Main!$N$8</f>
         <v>43760.256000000008</v>
       </c>
       <c r="J21" s="13">
-        <f>+[24]Main!$N$14</f>
+        <f>+[20]Main!$N$14</f>
         <v>49396.022818172591</v>
       </c>
       <c r="K21" s="13">
-        <f>+SUM([24]Model!$F$28:$I$28)</f>
+        <f>+SUM([20]Model!$F$28:$I$28)</f>
         <v>3890.6999999999989</v>
       </c>
       <c r="L21" s="29">
@@ -2988,16 +3077,81 @@
         <v>12.866593672089859</v>
       </c>
       <c r="N21" s="19">
-        <f>+[24]Main!$N$6</f>
+        <f>+[20]Main!$N$6</f>
         <v>79.680000000000007</v>
       </c>
       <c r="O21" s="19">
-        <f>+[24]Main!$N$15</f>
+        <f>+[20]Main!$N$15</f>
         <v>89.941774978464281</v>
       </c>
       <c r="P21" s="14">
         <f>O21/N21</f>
         <v>1.1287873365771119</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="4">
+        <v>44983</v>
+      </c>
+      <c r="D22" s="30">
+        <v>44895</v>
+      </c>
+      <c r="E22" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="12">
+        <f>+[25]Main!$N$11</f>
+        <v>1828.46028</v>
+      </c>
+      <c r="I22" s="13">
+        <f>+[25]Main!$N$8</f>
+        <v>1946.07728</v>
+      </c>
+      <c r="J22" s="13">
+        <f>+[25]Main!$N$14</f>
+        <v>2173.7463596759726</v>
+      </c>
+      <c r="K22" s="13">
+        <f>SUM([25]Model!$F$28:$I$28)</f>
+        <v>226.52699999999987</v>
+      </c>
+      <c r="L22" s="29">
+        <f t="shared" si="1"/>
+        <v>3.5525845304560546</v>
+      </c>
+      <c r="M22" s="28">
+        <f t="shared" si="2"/>
+        <v>8.0717101272696024</v>
+      </c>
+      <c r="N22" s="19">
+        <f>+[25]Main!$N$6</f>
+        <v>30.52</v>
+      </c>
+      <c r="O22" s="19">
+        <f>+[25]Main!$N$15</f>
+        <v>34.090495572360147</v>
+      </c>
+      <c r="P22" s="14">
+        <f>O22/N22</f>
+        <v>1.1169887146906994</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3034,9 +3188,10 @@
     <hyperlink ref="F19" r:id="rId18" xr:uid="{9712A0F2-E276-4023-8E1C-20FFFF3D79AF}"/>
     <hyperlink ref="F20" r:id="rId19" xr:uid="{D51FB28B-25B5-4085-89BA-B30029424F9C}"/>
     <hyperlink ref="F21" r:id="rId20" xr:uid="{A5AEC059-A102-4726-A849-58E7EC9248D0}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{C57C69B0-2AD6-4678-BD43-7D4F057F81B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -3474,19 +3629,19 @@
         <v>33</v>
       </c>
       <c r="G6" s="12">
-        <f>+[20]Main!$J$8</f>
+        <f>+[21]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[20]Main!$J$18</f>
+        <f>+[21]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[20]Main!$J$3</f>
+        <f>+[21]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[20]Main!$J$19</f>
+        <f>+[21]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3769,19 +3924,19 @@
         <v>97</v>
       </c>
       <c r="G2" s="12">
-        <f>[21]Main!$O$8</f>
+        <f>[22]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[21]Main!$O$18</f>
+        <f>[22]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[21]Main!$O$3</f>
+        <f>[22]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[21]Main!$O$19</f>
+        <f>[22]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3809,19 +3964,19 @@
         <v>103</v>
       </c>
       <c r="G3" s="12">
-        <f>+[22]Main!$N$8</f>
+        <f>+[23]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[22]Main!$N$18</f>
+        <f>+[23]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[22]Main!$N$3</f>
+        <f>+[23]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[22]Main!$N$19</f>
+        <f>+[23]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3852,19 +4007,19 @@
         <v>108</v>
       </c>
       <c r="G4" s="12">
-        <f>[23]Main!$J$8</f>
+        <f>[24]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[23]Main!$J$18</f>
+        <f>[24]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[23]Main!$J$3</f>
+        <f>[24]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[23]Main!$J$19</f>
+        <f>[24]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2023Q1 DCF Update for DRHorton (DHI)
Undervalued.
Price target: $163.03
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C228F9-BE6B-495D-8349-03C6DDDA3E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CAF4E-8A7A-40C4-89A6-EF3C3C20CE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16545" yWindow="6030" windowWidth="27045" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="2055" yWindow="4560" windowWidth="27045" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
   <si>
     <t>Ticker</t>
   </si>
@@ -120,21 +120,12 @@
     <t>Analog Devices</t>
   </si>
   <si>
-    <t>On semi</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
     <t>22Q2</t>
   </si>
   <si>
-    <t>? First one need to 2 check</t>
-  </si>
-  <si>
-    <t>Low gross margin</t>
-  </si>
-  <si>
     <t>JWN</t>
   </si>
   <si>
@@ -337,9 +328,6 @@
   </si>
   <si>
     <t>Vehicle components</t>
-  </si>
-  <si>
-    <t>General electronics</t>
   </si>
   <si>
     <t>LQDT</t>
@@ -783,34 +771,59 @@
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="N3">
-            <v>76.150000000000006</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>31004.120000000003</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="N18">
-            <v>59674.776053903901</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="N19">
-            <v>170.11053607156185</v>
+        <row r="5">
+          <cell r="N5">
+            <v>91.49</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="N7">
+            <v>31490.857999999997</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>34568.657999999996</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>56115.999003056495</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>163.0331173825</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="15">
+          <cell r="L15">
+            <v>1874.0000000000005</v>
+          </cell>
+          <cell r="M15">
+            <v>2168.1</v>
+          </cell>
+          <cell r="N15">
+            <v>2046.4999999999977</v>
+          </cell>
+          <cell r="O15">
+            <v>1229.5</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1119,7 +1132,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1171,7 +1184,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1268,7 +1281,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1277,34 +1290,59 @@
 <file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="6">
+          <cell r="N6">
+            <v>30.52</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>1946.07728</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>1828.46028</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>2173.7463596759726</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>34.090495572360147</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="F28">
+            <v>52.289999999999864</v>
+          </cell>
+          <cell r="G28">
+            <v>55.844000000000015</v>
+          </cell>
+          <cell r="H28">
+            <v>72.525999999999996</v>
+          </cell>
+          <cell r="I28">
+            <v>45.867000000000004</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1320,23 +1358,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1356,23 +1394,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1392,23 +1430,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1421,59 +1459,34 @@
 <file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="6">
-          <cell r="N6">
-            <v>30.52</v>
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>1946.07728</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="N11">
-            <v>1828.46028</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>2173.7463596759726</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="N15">
-            <v>34.090495572360147</v>
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="28">
-          <cell r="F28">
-            <v>52.289999999999864</v>
-          </cell>
-          <cell r="G28">
-            <v>55.844000000000015</v>
-          </cell>
-          <cell r="H28">
-            <v>72.525999999999996</v>
-          </cell>
-          <cell r="I28">
-            <v>45.867000000000004</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2032,7 +2045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2057,16 +2070,16 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2078,55 +2091,55 @@
         <v>1</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="4">
         <v>44775</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" s="12">
         <f>[1]Main!$N$8</f>
@@ -2149,28 +2162,28 @@
         <v>4.733613984693994</v>
       </c>
       <c r="Q2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4">
         <v>44772</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H3" s="12">
         <f>[2]Main!$N$8</f>
@@ -2193,28 +2206,28 @@
         <v>4.3731421333760139</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4">
         <v>44773</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H4" s="12">
         <f>[3]Main!$N$8</f>
@@ -2239,10 +2252,10 @@
     </row>
     <row r="5" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4">
         <v>44773</v>
@@ -2252,10 +2265,10 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5" s="12">
         <f>[4]Main!$N$8</f>
@@ -2280,23 +2293,23 @@
     </row>
     <row r="6" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="4">
         <v>44773</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H6" s="12">
         <f>[5]Main!$N$8</f>
@@ -2321,23 +2334,23 @@
     </row>
     <row r="7" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="4">
         <v>44774</v>
       </c>
       <c r="D7" s="30"/>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H7" s="12">
         <f>[6]Main!$N$8</f>
@@ -2362,10 +2375,10 @@
     </row>
     <row r="8" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="4">
         <v>44774</v>
@@ -2375,10 +2388,10 @@
         <v>5</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H8" s="12">
         <f>[7]Main!$N$8</f>
@@ -2403,23 +2416,23 @@
     </row>
     <row r="9" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4">
         <v>44774</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H9" s="12">
         <f>[8]Main!$N$8</f>
@@ -2444,23 +2457,23 @@
     </row>
     <row r="10" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C10" s="4">
         <v>44775</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H10" s="12">
         <f>[9]Main!$N$8</f>
@@ -2485,23 +2498,23 @@
     </row>
     <row r="11" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11" s="4">
         <v>44775</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H11" s="12">
         <f>[10]Main!$N$8</f>
@@ -2526,23 +2539,23 @@
     </row>
     <row r="12" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4">
         <v>44775</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H12" s="12">
         <f>[11]Main!$N$8</f>
@@ -2565,57 +2578,75 @@
         <v>0.82662603606246043</v>
       </c>
       <c r="Q12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4">
-        <v>44778</v>
-      </c>
-      <c r="D13" s="30"/>
+        <v>44984</v>
+      </c>
+      <c r="D13" s="30">
+        <v>44951</v>
+      </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H13" s="12">
-        <f>[12]Main!$N$8</f>
-        <v>31004.120000000003</v>
+        <f>[12]Main!$N$10</f>
+        <v>34568.657999999996</v>
+      </c>
+      <c r="I13" s="13">
+        <f>+[12]Main!$N$7</f>
+        <v>31490.857999999997</v>
       </c>
       <c r="J13" s="13">
-        <f>[12]Main!$N$18</f>
-        <v>59674.776053903901</v>
+        <f>+[12]Main!$N$13</f>
+        <v>56115.999003056495</v>
+      </c>
+      <c r="K13" s="13">
+        <f>+SUM([12]Model!$L$15:$O$15)</f>
+        <v>7318.0999999999985</v>
+      </c>
+      <c r="L13" s="29">
+        <f t="shared" ref="L13:L22" si="1">K13/(J13/O13)</f>
+        <v>21.261185357350374</v>
+      </c>
+      <c r="M13" s="28">
+        <f t="shared" ref="M13:M22" si="2">H13/K13</f>
+        <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
-        <f>[12]Main!$N$3</f>
-        <v>76.150000000000006</v>
+        <f>[12]Main!$N$5</f>
+        <v>91.49</v>
       </c>
       <c r="O13" s="19">
-        <f>[12]Main!$N$19</f>
-        <v>170.11053607156185</v>
+        <f>+[12]Main!$N$14</f>
+        <v>163.0331173825</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="0"/>
-        <v>2.2338875386941806</v>
+        <v>1.7819774552683354</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C14" s="4">
         <v>44973</v>
@@ -2624,13 +2655,13 @@
         <v>44964</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H14" s="12">
         <f>[13]Main!$N$9</f>
@@ -2649,11 +2680,11 @@
         <v>642.59899999999948</v>
       </c>
       <c r="L14" s="29">
-        <f t="shared" ref="L14:L22" si="1">K14/(J14/O14)</f>
+        <f t="shared" si="1"/>
         <v>2.519294627770305</v>
       </c>
       <c r="M14" s="28">
-        <f t="shared" ref="M14:M22" si="2">H14/K14</f>
+        <f t="shared" si="2"/>
         <v>65.181544400162522</v>
       </c>
       <c r="N14" s="19">
@@ -2671,10 +2702,10 @@
     </row>
     <row r="15" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C15" s="4">
         <v>44972</v>
@@ -2683,13 +2714,13 @@
         <v>44916</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H15" s="12">
         <f>[14]Main!$N$9</f>
@@ -2730,10 +2761,10 @@
     </row>
     <row r="16" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C16" s="4">
         <v>44972</v>
@@ -2742,13 +2773,13 @@
         <v>44873</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F16" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" t="s">
         <v>117</v>
-      </c>
-      <c r="G16" t="s">
-        <v>121</v>
       </c>
       <c r="H16" s="12">
         <f>[15]Main!$N$9</f>
@@ -2788,10 +2819,10 @@
     </row>
     <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C17" s="4">
         <v>44972</v>
@@ -2800,13 +2831,13 @@
         <v>44867</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" t="s">
         <v>118</v>
-      </c>
-      <c r="G17" t="s">
-        <v>122</v>
       </c>
       <c r="H17" s="12">
         <f>[16]Main!$N$9</f>
@@ -2846,10 +2877,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C18" s="4">
         <v>44979</v>
@@ -2858,13 +2889,13 @@
         <v>44950</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="12">
         <f>[17]Main!$N$10</f>
@@ -2903,15 +2934,15 @@
         <v>0.86468027591094387</v>
       </c>
       <c r="Q18" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C19" s="4">
         <v>44980</v>
@@ -2920,7 +2951,7 @@
         <v>44972</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>17</v>
@@ -2965,15 +2996,15 @@
         <v>1.0148574813194355</v>
       </c>
       <c r="Q19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C20" s="4">
         <v>44981</v>
@@ -2982,13 +3013,13 @@
         <v>44963</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H20" s="12">
         <f>+[19]Main!$N$12</f>
@@ -3027,15 +3058,15 @@
         <v>1.0625269931140018</v>
       </c>
       <c r="Q20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C21" s="4">
         <v>44982</v>
@@ -3044,13 +3075,13 @@
         <v>44959</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H21" s="12">
         <f>+[20]Main!$N$11</f>
@@ -3089,15 +3120,15 @@
         <v>1.1287873365771119</v>
       </c>
       <c r="Q21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C22" s="4">
         <v>44983</v>
@@ -3106,28 +3137,28 @@
         <v>44895</v>
       </c>
       <c r="E22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="26" t="s">
-        <v>137</v>
-      </c>
       <c r="G22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H22" s="12">
-        <f>+[25]Main!$N$11</f>
+        <f>+[21]Main!$N$11</f>
         <v>1828.46028</v>
       </c>
       <c r="I22" s="13">
-        <f>+[25]Main!$N$8</f>
+        <f>+[21]Main!$N$8</f>
         <v>1946.07728</v>
       </c>
       <c r="J22" s="13">
-        <f>+[25]Main!$N$14</f>
+        <f>+[21]Main!$N$14</f>
         <v>2173.7463596759726</v>
       </c>
       <c r="K22" s="13">
-        <f>SUM([25]Model!$F$28:$I$28)</f>
+        <f>SUM([21]Model!$F$28:$I$28)</f>
         <v>226.52699999999987</v>
       </c>
       <c r="L22" s="29">
@@ -3139,11 +3170,11 @@
         <v>8.0717101272696024</v>
       </c>
       <c r="N22" s="19">
-        <f>+[25]Main!$N$6</f>
+        <f>+[21]Main!$N$6</f>
         <v>30.52</v>
       </c>
       <c r="O22" s="19">
-        <f>+[25]Main!$N$15</f>
+        <f>+[21]Main!$N$15</f>
         <v>34.090495572360147</v>
       </c>
       <c r="P22" s="14">
@@ -3151,7 +3182,7 @@
         <v>1.1169887146906994</v>
       </c>
       <c r="Q22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3197,10 +3228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F73C4D65-549C-45C8-8E56-0FDC50A5308E}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,7 +3252,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3233,129 +3264,90 @@
         <v>4</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="K1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>44776</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="22"/>
+      <c r="E2" s="22">
+        <v>44858</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="19"/>
-      <c r="K2" s="14"/>
+        <v>90</v>
+      </c>
+      <c r="G2" s="12">
+        <f>[9]Main!$N$8</f>
+        <v>6531.1078800000005</v>
+      </c>
+      <c r="H2" s="13">
+        <f>[9]Main!$N$18</f>
+        <v>8831.5667844635373</v>
+      </c>
+      <c r="I2" s="19">
+        <f>[9]Main!$N$3</f>
+        <v>260.32</v>
+      </c>
+      <c r="J2" s="19">
+        <f>[9]Main!$N$19</f>
+        <v>357.06180902658434</v>
+      </c>
+      <c r="K2" s="14">
+        <f t="shared" ref="K2" si="0">J2/I2</f>
+        <v>1.3716264944168115</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B3" s="5"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="I3" s="19"/>
       <c r="K3" s="14"/>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
+      <c r="B4" s="5"/>
       <c r="E4" s="22"/>
-      <c r="F4" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="I4" s="19"/>
       <c r="K4" s="14"/>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>44776</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="22">
-        <v>44858</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="12">
-        <f>[9]Main!$N$8</f>
-        <v>6531.1078800000005</v>
-      </c>
-      <c r="H5" s="13">
-        <f>[9]Main!$N$18</f>
-        <v>8831.5667844635373</v>
-      </c>
-      <c r="I5" s="19">
-        <f>[9]Main!$N$3</f>
-        <v>260.32</v>
-      </c>
-      <c r="J5" s="19">
-        <f>[9]Main!$N$19</f>
-        <v>357.06180902658434</v>
-      </c>
-      <c r="K5" s="14">
-        <f t="shared" ref="K5" si="0">J5/I5</f>
-        <v>1.3716264944168115</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="E5" s="22"/>
+      <c r="I5" s="19"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -3384,28 +3376,7 @@
       <c r="E9" s="22"/>
       <c r="I9" s="19"/>
       <c r="K9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="E10" s="22"/>
-      <c r="I10" s="19"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="E11" s="22"/>
-      <c r="I11" s="19"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="E12" s="22"/>
-      <c r="I12" s="19"/>
-      <c r="K12" s="14"/>
-      <c r="N12" s="1"/>
+      <c r="N9" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
@@ -3420,7 +3391,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K4 K6:K1048576">
+  <conditionalFormatting sqref="K3:K1048576 K1">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3432,7 +3403,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
+  <conditionalFormatting sqref="K2">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3445,10 +3416,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{2EB6F67C-0D9B-4ECF-9716-4DBD14C41168}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{BFD78B41-26C5-4F62-86C3-CB6F80A7C7C7}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{2FECCCE6-9678-48B4-953C-D18796E68957}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{04E6DBBA-9A36-417F-9821-390225E2FD6D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{04E6DBBA-9A36-417F-9821-390225E2FD6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3459,7 +3427,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,7 +3448,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3492,28 +3460,28 @@
         <v>4</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3527,39 +3495,39 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" s="23"/>
       <c r="J2" s="24"/>
       <c r="K2" s="14"/>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" s="19"/>
       <c r="J3" s="25"/>
       <c r="K3" s="14"/>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3573,19 +3541,19 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I4" s="23"/>
       <c r="J4" s="25"/>
       <c r="K4" s="14"/>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3600,15 +3568,15 @@
         <v>5</v>
       </c>
       <c r="E5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="19"/>
       <c r="K5" s="14"/>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3616,32 +3584,32 @@
         <v>44789</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[21]Main!$J$8</f>
+        <f>+[22]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[21]Main!$J$18</f>
+        <f>+[22]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[21]Main!$J$3</f>
+        <f>+[22]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[21]Main!$J$19</f>
+        <f>+[22]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -3667,43 +3635,43 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8" s="19"/>
       <c r="K8" s="14"/>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I9" s="19"/>
       <c r="K9" s="14"/>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3718,15 +3686,15 @@
         <v>5</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I10" s="19"/>
       <c r="K10" s="14"/>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3868,7 +3836,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3880,28 +3848,28 @@
         <v>4</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3909,34 +3877,34 @@
         <v>44777</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="22">
         <v>44869</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[22]Main!$O$8</f>
+        <f>[23]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[22]Main!$O$18</f>
+        <f>[23]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[22]Main!$O$3</f>
+        <f>[23]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[22]Main!$O$19</f>
+        <f>[23]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -3949,34 +3917,34 @@
         <v>44777</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="22">
         <v>44868</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[23]Main!$N$8</f>
+        <f>+[24]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[23]Main!$N$18</f>
+        <f>+[24]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[23]Main!$N$3</f>
+        <f>+[24]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[23]Main!$N$19</f>
+        <f>+[24]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -3984,7 +3952,7 @@
         <v>0.21332181544998316</v>
       </c>
       <c r="L3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3992,34 +3960,34 @@
         <v>44779</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="22">
         <v>44832</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[24]Main!$J$8</f>
+        <f>[25]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[24]Main!$J$18</f>
+        <f>[25]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[24]Main!$J$3</f>
+        <f>[25]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[24]Main!$J$19</f>
+        <f>[25]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">
@@ -4037,7 +4005,7 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E6" s="22"/>
       <c r="I6" s="19"/>

</xml_diff>

<commit_message>
2022Q4 DCF for OldDominionFreightLine (ODFL)
Fairly valued
Price target: $305.59
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E921A04D-DDA3-481F-947A-EC487747FAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8BCA4C-C7AE-47D6-9F7A-649238D16147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="5055" windowWidth="27045" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="18840" yWindow="5010" windowWidth="29565" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
   <si>
     <t>Ticker</t>
   </si>
@@ -475,6 +476,15 @@
   </si>
   <si>
     <t>100% fab outsourced, is the 2023Q3 acquisition bullish?</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>Trucking</t>
+  </si>
+  <si>
+    <t>ODFL</t>
   </si>
 </sst>
 </file>
@@ -875,7 +885,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -927,7 +937,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -993,7 +1003,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1507,6 +1517,63 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Dash"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Old Dominion Freight Line</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>352.95</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>39650.402999999998</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>39621.008000000002</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>34330.520064169796</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>305.59480206667075</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="32">
+          <cell r="T32">
+            <v>2116.6350000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2061,11 +2128,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2641,11 +2708,11 @@
         <v>7318.0999999999985</v>
       </c>
       <c r="L13" s="29">
-        <f t="shared" ref="L13:L22" si="1">K13/(J13/O13)</f>
+        <f t="shared" ref="L13:L23" si="1">K13/(J13/O13)</f>
         <v>21.261185357350374</v>
       </c>
       <c r="M13" s="28">
-        <f t="shared" ref="M13:M22" si="2">H13/K13</f>
+        <f t="shared" ref="M13:M23" si="2">H13/K13</f>
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
@@ -3205,6 +3272,66 @@
       </c>
       <c r="Q22" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="4">
+        <v>44991</v>
+      </c>
+      <c r="D23" s="30">
+        <v>44958</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" t="str">
+        <f>+[26]Main!$N$4</f>
+        <v>Old Dominion Freight Line</v>
+      </c>
+      <c r="H23" s="12">
+        <f>+[26]Main!$N$11</f>
+        <v>39621.008000000002</v>
+      </c>
+      <c r="I23" s="13">
+        <f>+[26]Main!$N$8</f>
+        <v>39650.402999999998</v>
+      </c>
+      <c r="J23" s="13">
+        <f>+[26]Main!$N$14</f>
+        <v>34330.520064169796</v>
+      </c>
+      <c r="K23" s="13">
+        <f>+[26]Model!$T$32</f>
+        <v>2116.6350000000002</v>
+      </c>
+      <c r="L23" s="29">
+        <f t="shared" si="1"/>
+        <v>18.841329891401102</v>
+      </c>
+      <c r="M23" s="28">
+        <f t="shared" si="2"/>
+        <v>18.718866502727206</v>
+      </c>
+      <c r="N23" s="19">
+        <f>+[26]Main!$N$6</f>
+        <v>352.95</v>
+      </c>
+      <c r="O23" s="19">
+        <f>+[26]Main!$N$15</f>
+        <v>305.59480206667075</v>
+      </c>
+      <c r="P23" s="14">
+        <f>O23/N23</f>
+        <v>0.8658302934315647</v>
       </c>
     </row>
   </sheetData>
@@ -3242,9 +3369,10 @@
     <hyperlink ref="F20" r:id="rId19" xr:uid="{D51FB28B-25B5-4085-89BA-B30029424F9C}"/>
     <hyperlink ref="F21" r:id="rId20" xr:uid="{A5AEC059-A102-4726-A849-58E7EC9248D0}"/>
     <hyperlink ref="F22" r:id="rId21" xr:uid="{C57C69B0-2AD6-4678-BD43-7D4F057F81B0}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{7C4AE6AF-6F0A-4FAE-A5D5-4E5F41E85210}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2022Q4 DCF for Saia (SAIA)
Fairly valued
Price target: $289.77
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8BCA4C-C7AE-47D6-9F7A-649238D16147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E663B34D-C969-4848-8F1E-7B385FD5E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="5010" windowWidth="29565" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="22965" yWindow="4350" windowWidth="25455" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
     <externalReference r:id="rId30"/>
+    <externalReference r:id="rId31"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="144">
   <si>
     <t>Ticker</t>
   </si>
@@ -485,6 +486,9 @@
   </si>
   <si>
     <t>ODFL</t>
+  </si>
+  <si>
+    <t>SAIA</t>
   </si>
 </sst>
 </file>
@@ -1381,34 +1385,55 @@
 <file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Old Dominion Freight Line</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>352.95</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>39650.402999999998</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>39621.008000000002</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>34330.520064169796</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>305.59480206667075</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="32">
+          <cell r="T32">
+            <v>2116.6350000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1424,23 +1449,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1460,23 +1485,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1496,23 +1521,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1523,6 +1548,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1535,41 +1596,51 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="2">
+          <cell r="N2">
+            <v>44992</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>Old Dominion Freight Line</v>
+            <v>Saia</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>352.95</v>
+            <v>288.77</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>39650.402999999998</v>
+            <v>7658.1803999999993</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>39621.008000000002</v>
+            <v>7707.5203999999994</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>34330.520064169796</v>
+            <v>7684.7281871497207</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>305.59480206667075</v>
+            <v>289.77104778090956</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="32">
-          <cell r="T32">
-            <v>2116.6350000000002</v>
+        <row r="1">
+          <cell r="J1">
+            <v>44595</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="T28">
+            <v>627.74999999999977</v>
           </cell>
         </row>
       </sheetData>
@@ -2128,11 +2199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2708,11 +2779,11 @@
         <v>7318.0999999999985</v>
       </c>
       <c r="L13" s="29">
-        <f t="shared" ref="L13:L23" si="1">K13/(J13/O13)</f>
+        <f t="shared" ref="L13:L24" si="1">K13/(J13/O13)</f>
         <v>21.261185357350374</v>
       </c>
       <c r="M13" s="28">
-        <f t="shared" ref="M13:M23" si="2">H13/K13</f>
+        <f t="shared" ref="M13:M24" si="2">H13/K13</f>
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
@@ -3019,7 +3090,7 @@
         <v>146.82271084967829</v>
       </c>
       <c r="P18" s="14">
-        <f>O18/N18</f>
+        <f t="shared" ref="P18:P24" si="3">O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
       <c r="Q18" t="s">
@@ -3081,7 +3152,7 @@
         <v>188.40829140695323</v>
       </c>
       <c r="P19" s="14">
-        <f>O19/N19</f>
+        <f t="shared" si="3"/>
         <v>1.0148574813194355</v>
       </c>
       <c r="Q19" t="s">
@@ -3143,7 +3214,7 @@
         <v>81.049559034736063</v>
       </c>
       <c r="P20" s="14">
-        <f>O20/N20</f>
+        <f t="shared" si="3"/>
         <v>1.0625269931140018</v>
       </c>
       <c r="Q20" t="s">
@@ -3205,7 +3276,7 @@
         <v>89.941774978464281</v>
       </c>
       <c r="P21" s="14">
-        <f>O21/N21</f>
+        <f t="shared" si="3"/>
         <v>1.1287873365771119</v>
       </c>
       <c r="Q21" t="s">
@@ -3267,7 +3338,7 @@
         <v>34.090495572360147</v>
       </c>
       <c r="P22" s="14">
-        <f>O22/N22</f>
+        <f t="shared" si="3"/>
         <v>1.1169887146906994</v>
       </c>
       <c r="Q22" t="s">
@@ -3294,23 +3365,23 @@
         <v>142</v>
       </c>
       <c r="G23" t="str">
-        <f>+[26]Main!$N$4</f>
+        <f>+[22]Main!$N$4</f>
         <v>Old Dominion Freight Line</v>
       </c>
       <c r="H23" s="12">
-        <f>+[26]Main!$N$11</f>
+        <f>+[22]Main!$N$11</f>
         <v>39621.008000000002</v>
       </c>
       <c r="I23" s="13">
-        <f>+[26]Main!$N$8</f>
+        <f>+[22]Main!$N$8</f>
         <v>39650.402999999998</v>
       </c>
       <c r="J23" s="13">
-        <f>+[26]Main!$N$14</f>
+        <f>+[22]Main!$N$14</f>
         <v>34330.520064169796</v>
       </c>
       <c r="K23" s="13">
-        <f>+[26]Model!$T$32</f>
+        <f>+[22]Model!$T$32</f>
         <v>2116.6350000000002</v>
       </c>
       <c r="L23" s="29">
@@ -3322,16 +3393,78 @@
         <v>18.718866502727206</v>
       </c>
       <c r="N23" s="19">
-        <f>+[26]Main!$N$6</f>
+        <f>+[22]Main!$N$6</f>
         <v>352.95</v>
       </c>
       <c r="O23" s="19">
-        <f>+[26]Main!$N$15</f>
+        <f>+[22]Main!$N$15</f>
         <v>305.59480206667075</v>
       </c>
       <c r="P23" s="14">
-        <f>O23/N23</f>
+        <f t="shared" si="3"/>
         <v>0.8658302934315647</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="4">
+        <f>+[27]Main!$N$2</f>
+        <v>44992</v>
+      </c>
+      <c r="D24" s="30">
+        <f>+[27]Model!$J$1</f>
+        <v>44595</v>
+      </c>
+      <c r="E24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" t="str">
+        <f>+[27]Main!$N$4</f>
+        <v>Saia</v>
+      </c>
+      <c r="H24" s="12">
+        <f>+[27]Main!$N$11</f>
+        <v>7707.5203999999994</v>
+      </c>
+      <c r="I24" s="13">
+        <f>+[27]Main!$N$8</f>
+        <v>7658.1803999999993</v>
+      </c>
+      <c r="J24" s="13">
+        <f>+[27]Main!$N$14</f>
+        <v>7684.7281871497207</v>
+      </c>
+      <c r="K24" s="13">
+        <f>+[27]Model!$T$28</f>
+        <v>627.74999999999977</v>
+      </c>
+      <c r="L24" s="29">
+        <f t="shared" si="1"/>
+        <v>23.670814479638004</v>
+      </c>
+      <c r="M24" s="28">
+        <f t="shared" si="2"/>
+        <v>12.278009398645962</v>
+      </c>
+      <c r="N24" s="19">
+        <f>+[27]Main!$N$6</f>
+        <v>288.77</v>
+      </c>
+      <c r="O24" s="19">
+        <f>+[27]Main!$N$15</f>
+        <v>289.77104778090956</v>
+      </c>
+      <c r="P24" s="14">
+        <f t="shared" si="3"/>
+        <v>1.0034665920314076</v>
       </c>
     </row>
   </sheetData>
@@ -3370,9 +3503,10 @@
     <hyperlink ref="F21" r:id="rId20" xr:uid="{A5AEC059-A102-4726-A849-58E7EC9248D0}"/>
     <hyperlink ref="F22" r:id="rId21" xr:uid="{C57C69B0-2AD6-4678-BD43-7D4F057F81B0}"/>
     <hyperlink ref="F23" r:id="rId22" xr:uid="{7C4AE6AF-6F0A-4FAE-A5D5-4E5F41E85210}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{4633F666-AB4C-44FF-ACE3-52918E85357E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -3747,19 +3881,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[22]Main!$J$8</f>
+        <f>+[23]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[22]Main!$J$18</f>
+        <f>+[23]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[22]Main!$J$3</f>
+        <f>+[23]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[22]Main!$J$19</f>
+        <f>+[23]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -4042,19 +4176,19 @@
         <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[23]Main!$O$8</f>
+        <f>[24]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[23]Main!$O$18</f>
+        <f>[24]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[23]Main!$O$3</f>
+        <f>[24]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[23]Main!$O$19</f>
+        <f>[24]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -4082,19 +4216,19 @@
         <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[24]Main!$N$8</f>
+        <f>+[25]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[24]Main!$N$18</f>
+        <f>+[25]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[24]Main!$N$3</f>
+        <f>+[25]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[24]Main!$N$19</f>
+        <f>+[25]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -4125,19 +4259,19 @@
         <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[25]Main!$J$8</f>
+        <f>[26]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[25]Main!$J$18</f>
+        <f>[26]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[25]Main!$J$3</f>
+        <f>[26]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[25]Main!$J$19</f>
+        <f>[26]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2022Q4 DCF for PAMTransportServices (PTSI)
Unvalued by a lot, will be chucking a good amount into this
Price target: $43.27
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E663B34D-C969-4848-8F1E-7B385FD5E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23716492-6EA5-4E5E-9141-B7FFF247965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22965" yWindow="4350" windowWidth="25455" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="15240" yWindow="5235" windowWidth="12570" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <externalReference r:id="rId29"/>
     <externalReference r:id="rId30"/>
     <externalReference r:id="rId31"/>
+    <externalReference r:id="rId32"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
   <si>
     <t>Ticker</t>
   </si>
@@ -489,6 +490,9 @@
   </si>
   <si>
     <t>SAIA</t>
+  </si>
+  <si>
+    <t>PTSI</t>
   </si>
 </sst>
 </file>
@@ -1442,34 +1446,65 @@
 <file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44992</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Saia</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>288.77</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>7658.1803999999993</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>7707.5203999999994</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>7684.7281871497207</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>289.77104778090956</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44595</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="T28">
+            <v>627.74999999999977</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1485,23 +1520,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1521,23 +1556,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1557,23 +1592,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="N8">
+            <v>217.09325999999999</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="N18">
+            <v>42.225188935657137</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
@@ -1584,6 +1619,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1603,48 +1674,48 @@
         </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>Saia</v>
+            <v>P.A.M. Transportation Services</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>288.77</v>
+            <v>29.24</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>7658.1803999999993</v>
+            <v>656.02864</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>7707.5203999999994</v>
+            <v>853.44364000000007</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>7684.7281871497207</v>
+            <v>970.90412687107221</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>289.77104778090956</v>
+            <v>43.274386114774124</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="J1">
-            <v>44595</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="T28">
-            <v>627.74999999999977</v>
+            <v>44605</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="T31">
+            <v>186.68</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2199,11 +2270,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2779,11 +2850,11 @@
         <v>7318.0999999999985</v>
       </c>
       <c r="L13" s="29">
-        <f t="shared" ref="L13:L24" si="1">K13/(J13/O13)</f>
+        <f t="shared" ref="L13:L25" si="1">K13/(J13/O13)</f>
         <v>21.261185357350374</v>
       </c>
       <c r="M13" s="28">
-        <f t="shared" ref="M13:M24" si="2">H13/K13</f>
+        <f t="shared" ref="M13:M25" si="2">H13/K13</f>
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
@@ -3090,7 +3161,7 @@
         <v>146.82271084967829</v>
       </c>
       <c r="P18" s="14">
-        <f t="shared" ref="P18:P24" si="3">O18/N18</f>
+        <f t="shared" ref="P18:P25" si="3">O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
       <c r="Q18" t="s">
@@ -3413,11 +3484,11 @@
         <v>141</v>
       </c>
       <c r="C24" s="4">
-        <f>+[27]Main!$N$2</f>
+        <f>+[23]Main!$N$2</f>
         <v>44992</v>
       </c>
       <c r="D24" s="30">
-        <f>+[27]Model!$J$1</f>
+        <f>+[23]Model!$J$1</f>
         <v>44595</v>
       </c>
       <c r="E24" t="s">
@@ -3427,23 +3498,23 @@
         <v>143</v>
       </c>
       <c r="G24" t="str">
-        <f>+[27]Main!$N$4</f>
+        <f>+[23]Main!$N$4</f>
         <v>Saia</v>
       </c>
       <c r="H24" s="12">
-        <f>+[27]Main!$N$11</f>
+        <f>+[23]Main!$N$11</f>
         <v>7707.5203999999994</v>
       </c>
       <c r="I24" s="13">
-        <f>+[27]Main!$N$8</f>
+        <f>+[23]Main!$N$8</f>
         <v>7658.1803999999993</v>
       </c>
       <c r="J24" s="13">
-        <f>+[27]Main!$N$14</f>
+        <f>+[23]Main!$N$14</f>
         <v>7684.7281871497207</v>
       </c>
       <c r="K24" s="13">
-        <f>+[27]Model!$T$28</f>
+        <f>+[23]Model!$T$28</f>
         <v>627.74999999999977</v>
       </c>
       <c r="L24" s="29">
@@ -3455,16 +3526,78 @@
         <v>12.278009398645962</v>
       </c>
       <c r="N24" s="19">
-        <f>+[27]Main!$N$6</f>
+        <f>+[23]Main!$N$6</f>
         <v>288.77</v>
       </c>
       <c r="O24" s="19">
-        <f>+[27]Main!$N$15</f>
+        <f>+[23]Main!$N$15</f>
         <v>289.77104778090956</v>
       </c>
       <c r="P24" s="14">
         <f t="shared" si="3"/>
         <v>1.0034665920314076</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="4">
+        <f>+[28]Main!$N$2</f>
+        <v>44992</v>
+      </c>
+      <c r="D25" s="30">
+        <f>+[28]Model!$J$1</f>
+        <v>44605</v>
+      </c>
+      <c r="E25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" t="str">
+        <f>+[28]Main!$N$4</f>
+        <v>P.A.M. Transportation Services</v>
+      </c>
+      <c r="H25" s="12">
+        <f>+[28]Main!$N$11</f>
+        <v>853.44364000000007</v>
+      </c>
+      <c r="I25" s="13">
+        <f>+[28]Main!$N$8</f>
+        <v>656.02864</v>
+      </c>
+      <c r="J25" s="13">
+        <f>+[28]Main!$N$14</f>
+        <v>970.90412687107221</v>
+      </c>
+      <c r="K25" s="13">
+        <f>+[28]Model!$T$31</f>
+        <v>186.68</v>
+      </c>
+      <c r="L25" s="29">
+        <f t="shared" si="1"/>
+        <v>8.320556248885719</v>
+      </c>
+      <c r="M25" s="28">
+        <f t="shared" si="2"/>
+        <v>4.571692950503536</v>
+      </c>
+      <c r="N25" s="19">
+        <f>+[28]Main!$N$6</f>
+        <v>29.24</v>
+      </c>
+      <c r="O25" s="19">
+        <f>+[28]Main!$N$15</f>
+        <v>43.274386114774124</v>
+      </c>
+      <c r="P25" s="14">
+        <f t="shared" si="3"/>
+        <v>1.4799721653479523</v>
       </c>
     </row>
   </sheetData>
@@ -3504,9 +3637,10 @@
     <hyperlink ref="F22" r:id="rId21" xr:uid="{C57C69B0-2AD6-4678-BD43-7D4F057F81B0}"/>
     <hyperlink ref="F23" r:id="rId22" xr:uid="{7C4AE6AF-6F0A-4FAE-A5D5-4E5F41E85210}"/>
     <hyperlink ref="F24" r:id="rId23" xr:uid="{4633F666-AB4C-44FF-ACE3-52918E85357E}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{B7CF3F61-BFC6-41D5-8919-5EDA0850C31F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId24"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -3711,7 +3845,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,19 +4015,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[23]Main!$J$8</f>
+        <f>+[24]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[23]Main!$J$18</f>
+        <f>+[24]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[23]Main!$J$3</f>
+        <f>+[24]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[23]Main!$J$19</f>
+        <f>+[24]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -4176,19 +4310,19 @@
         <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[24]Main!$O$8</f>
+        <f>[25]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[24]Main!$O$18</f>
+        <f>[25]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[24]Main!$O$3</f>
+        <f>[25]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[24]Main!$O$19</f>
+        <f>[25]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -4216,19 +4350,19 @@
         <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[25]Main!$N$8</f>
+        <f>+[26]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[25]Main!$N$18</f>
+        <f>+[26]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[25]Main!$N$3</f>
+        <f>+[26]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[25]Main!$N$19</f>
+        <f>+[26]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -4259,19 +4393,19 @@
         <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[26]Main!$J$8</f>
+        <f>[27]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[26]Main!$J$18</f>
+        <f>[27]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[26]Main!$J$3</f>
+        <f>[27]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[26]Main!$J$19</f>
+        <f>[27]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2022Q4 DCF for Covenant Logistics Group (CVLG)
Undervalued, Strong Buy. I tried everything to kill this corporation, but they survived, even at 2.6% operating margin.
Price target:  $44.99
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23716492-6EA5-4E5E-9141-B7FFF247965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB559D-EE2C-406C-9EE3-4B71181FD1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="5235" windowWidth="12570" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="10620" yWindow="6240" windowWidth="37335" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,8 @@
     <externalReference r:id="rId30"/>
     <externalReference r:id="rId31"/>
     <externalReference r:id="rId32"/>
+    <externalReference r:id="rId33"/>
+    <externalReference r:id="rId34"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
   <si>
     <t>Ticker</t>
   </si>
@@ -493,6 +495,24 @@
   </si>
   <si>
     <t>PTSI</t>
+  </si>
+  <si>
+    <t>98% LTL (less then truckload)</t>
+  </si>
+  <si>
+    <t>96% LTL</t>
+  </si>
+  <si>
+    <t>CVLG</t>
+  </si>
+  <si>
+    <t>Low LTL, 4.0% op margin</t>
+  </si>
+  <si>
+    <t>Low LTL, I tried everything I could to kill these guys, and even at a 2.6% op margin they survived</t>
+  </si>
+  <si>
+    <t>HTLD</t>
   </si>
 </sst>
 </file>
@@ -592,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -660,6 +680,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1513,34 +1534,65 @@
 <file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44992</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>P.A.M. Transportation Services</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>29.24</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>656.02864</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>853.44364000000007</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>970.90412687107221</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>43.274386114774124</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44605</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="T31">
+            <v>186.68</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1549,34 +1601,65 @@
 <file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44992</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Covenant Logistics Group</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>35.369999999999997</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="N8">
+            <v>530.76221999999996</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>635.8222199999999</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>675.0558523176453</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>44.985729196164556</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44951</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="T35">
+            <v>178.19999999999982</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1592,23 +1675,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1628,23 +1711,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1657,65 +1740,70 @@
 <file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="N2">
-            <v>44992</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="N4" t="str">
-            <v>P.A.M. Transportation Services</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>29.24</v>
+        <row r="3">
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>656.02864</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="N11">
-            <v>853.44364000000007</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>970.90412687107221</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="N15">
-            <v>43.274386114774124</v>
+            <v>217.09325999999999</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>42.225188935657137</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="J1">
-            <v>44605</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="T31">
-            <v>186.68</v>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1752,6 +1840,73 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Dash"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="N2">
+            <v>44993</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Heartland Express</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>16.260000000000002</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>1283.5806600000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>1763.72066</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>1294.1990734380452</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>16.394510754082734</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="N17">
+            <v>321.39600000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44595</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2270,11 +2425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2850,11 +3005,11 @@
         <v>7318.0999999999985</v>
       </c>
       <c r="L13" s="29">
-        <f t="shared" ref="L13:L25" si="1">K13/(J13/O13)</f>
+        <f t="shared" ref="L13:L26" si="1">K13/(J13/O13)</f>
         <v>21.261185357350374</v>
       </c>
       <c r="M13" s="28">
-        <f t="shared" ref="M13:M25" si="2">H13/K13</f>
+        <f t="shared" ref="M13:M26" si="2">H13/K13</f>
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
@@ -3161,7 +3316,7 @@
         <v>146.82271084967829</v>
       </c>
       <c r="P18" s="14">
-        <f t="shared" ref="P18:P25" si="3">O18/N18</f>
+        <f t="shared" ref="P18:P27" si="3">O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
       <c r="Q18" t="s">
@@ -3475,8 +3630,11 @@
         <f t="shared" si="3"/>
         <v>0.8658302934315647</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -3537,8 +3695,11 @@
         <f t="shared" si="3"/>
         <v>1.0034665920314076</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -3546,11 +3707,11 @@
         <v>141</v>
       </c>
       <c r="C25" s="4">
-        <f>+[28]Main!$N$2</f>
+        <f>+[24]Main!$N$2</f>
         <v>44992</v>
       </c>
       <c r="D25" s="30">
-        <f>+[28]Model!$J$1</f>
+        <f>+[24]Model!$J$1</f>
         <v>44605</v>
       </c>
       <c r="E25" t="s">
@@ -3560,23 +3721,23 @@
         <v>144</v>
       </c>
       <c r="G25" t="str">
-        <f>+[28]Main!$N$4</f>
+        <f>+[24]Main!$N$4</f>
         <v>P.A.M. Transportation Services</v>
       </c>
       <c r="H25" s="12">
-        <f>+[28]Main!$N$11</f>
+        <f>+[24]Main!$N$11</f>
         <v>853.44364000000007</v>
       </c>
       <c r="I25" s="13">
-        <f>+[28]Main!$N$8</f>
+        <f>+[24]Main!$N$8</f>
         <v>656.02864</v>
       </c>
       <c r="J25" s="13">
-        <f>+[28]Main!$N$14</f>
+        <f>+[24]Main!$N$14</f>
         <v>970.90412687107221</v>
       </c>
       <c r="K25" s="13">
-        <f>+[28]Model!$T$31</f>
+        <f>+[24]Model!$T$31</f>
         <v>186.68</v>
       </c>
       <c r="L25" s="29">
@@ -3588,16 +3749,154 @@
         <v>4.571692950503536</v>
       </c>
       <c r="N25" s="19">
-        <f>+[28]Main!$N$6</f>
+        <f>+[24]Main!$N$6</f>
         <v>29.24</v>
       </c>
       <c r="O25" s="19">
-        <f>+[28]Main!$N$15</f>
+        <f>+[24]Main!$N$15</f>
         <v>43.274386114774124</v>
       </c>
       <c r="P25" s="14">
         <f t="shared" si="3"/>
         <v>1.4799721653479523</v>
+      </c>
+      <c r="Q25" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="4">
+        <f>+[25]Main!$N$2</f>
+        <v>44992</v>
+      </c>
+      <c r="D26" s="30">
+        <f>+[25]Model!$J$1</f>
+        <v>44951</v>
+      </c>
+      <c r="E26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" t="str">
+        <f>+[25]Main!$N$4</f>
+        <v>Covenant Logistics Group</v>
+      </c>
+      <c r="H26" s="12">
+        <f>+[25]Main!$N$11</f>
+        <v>635.8222199999999</v>
+      </c>
+      <c r="I26" s="13">
+        <f>+[25]Main!$N$8</f>
+        <v>530.76221999999996</v>
+      </c>
+      <c r="J26" s="13">
+        <f>+[25]Main!$N$14</f>
+        <v>675.0558523176453</v>
+      </c>
+      <c r="K26" s="13">
+        <f>+[25]Model!$T$35</f>
+        <v>178.19999999999982</v>
+      </c>
+      <c r="L26" s="29">
+        <f t="shared" si="1"/>
+        <v>11.875249900039972</v>
+      </c>
+      <c r="M26" s="28">
+        <f>H26/K26</f>
+        <v>3.5680259259259288</v>
+      </c>
+      <c r="N26" s="19">
+        <f>+[25]Main!$N$6</f>
+        <v>35.369999999999997</v>
+      </c>
+      <c r="O26" s="19">
+        <f>+[25]Main!$N$15</f>
+        <v>44.985729196164556</v>
+      </c>
+      <c r="P26" s="14">
+        <f t="shared" si="3"/>
+        <v>1.2718611590660038</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="4">
+        <f>+[30]Main!$N$2</f>
+        <v>44993</v>
+      </c>
+      <c r="D27" s="30">
+        <f>+[30]Model!$J$1</f>
+        <v>44595</v>
+      </c>
+      <c r="E27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" t="str">
+        <f>+[30]Main!$N$4</f>
+        <v>Heartland Express</v>
+      </c>
+      <c r="H27" s="12">
+        <f>+[30]Main!$N$11</f>
+        <v>1763.72066</v>
+      </c>
+      <c r="I27" s="13">
+        <f>+[30]Main!$N$8</f>
+        <v>1283.5806600000001</v>
+      </c>
+      <c r="J27" s="13">
+        <f>+[30]Main!$N$14</f>
+        <v>1294.1990734380452</v>
+      </c>
+      <c r="K27" s="13">
+        <f>+[30]Main!$N$17</f>
+        <v>321.39600000000002</v>
+      </c>
+      <c r="L27" s="29">
+        <f t="shared" ref="L27" si="4">K27/(J27/O27)</f>
+        <v>4.0713444217833574</v>
+      </c>
+      <c r="M27" s="28">
+        <f>H27/K27</f>
+        <v>5.4876870278410435</v>
+      </c>
+      <c r="N27" s="19">
+        <f>+[30]Main!$N$6</f>
+        <v>16.260000000000002</v>
+      </c>
+      <c r="O27" s="19">
+        <f>+[30]Main!$N$15</f>
+        <v>16.394510754082734</v>
+      </c>
+      <c r="P27" s="14">
+        <f t="shared" si="3"/>
+        <v>1.008272494101029</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3638,9 +3937,11 @@
     <hyperlink ref="F23" r:id="rId22" xr:uid="{7C4AE6AF-6F0A-4FAE-A5D5-4E5F41E85210}"/>
     <hyperlink ref="F24" r:id="rId23" xr:uid="{4633F666-AB4C-44FF-ACE3-52918E85357E}"/>
     <hyperlink ref="F25" r:id="rId24" xr:uid="{B7CF3F61-BFC6-41D5-8919-5EDA0850C31F}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{2F373320-D823-4882-B676-2DA2483444D3}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{3EE9ACF3-C9F0-41B1-A950-5743DB0F0BEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -4015,19 +4316,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[24]Main!$J$8</f>
+        <f>+[26]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[24]Main!$J$18</f>
+        <f>+[26]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[24]Main!$J$3</f>
+        <f>+[26]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[24]Main!$J$19</f>
+        <f>+[26]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -4310,19 +4611,19 @@
         <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[25]Main!$O$8</f>
+        <f>[27]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[25]Main!$O$18</f>
+        <f>[27]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[25]Main!$O$3</f>
+        <f>[27]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[25]Main!$O$19</f>
+        <f>[27]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -4350,19 +4651,19 @@
         <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[26]Main!$N$8</f>
+        <f>+[28]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[26]Main!$N$18</f>
+        <f>+[28]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[26]Main!$N$3</f>
+        <f>+[28]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[26]Main!$N$19</f>
+        <f>+[28]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -4393,19 +4694,19 @@
         <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[27]Main!$J$8</f>
+        <f>[29]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[27]Main!$J$18</f>
+        <f>[29]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[27]Main!$J$3</f>
+        <f>[29]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[27]Main!$J$19</f>
+        <f>[29]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2022Q4 DCF for Heartland Express (HTLD)
Fairly valued.
Price target:  $16.39
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB559D-EE2C-406C-9EE3-4B71181FD1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D7002-0BD9-4D4E-AAC7-663CBD54776D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10620" yWindow="6240" windowWidth="37335" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
@@ -1906,7 +1906,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2429,7 +2429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2022Q4 DCF for ArcBest (ARCB)
Potential buy.
Price target: $125.43
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D7002-0BD9-4D4E-AAC7-663CBD54776D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B27EA-7E80-4BDB-BF06-DCDF4F809521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="6240" windowWidth="37335" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="13560" yWindow="6210" windowWidth="30720" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,7 @@
     <externalReference r:id="rId32"/>
     <externalReference r:id="rId33"/>
     <externalReference r:id="rId34"/>
+    <externalReference r:id="rId35"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
   <si>
     <t>Ticker</t>
   </si>
@@ -513,19 +514,29 @@
   </si>
   <si>
     <t>HTLD</t>
+  </si>
+  <si>
+    <t>ARCB</t>
+  </si>
+  <si>
+    <t>Trying to be a tech company, I tried to kill these guys, and even at a 2.5% op margin they survived</t>
+  </si>
+  <si>
+    <t>This is a mid company, 5.8% margin and still no upside</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0\x"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00\x"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +548,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -612,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -673,14 +691,17 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -862,7 +883,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -914,7 +935,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -966,7 +987,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1032,7 +1053,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1077,8 +1098,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1130,7 +1151,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1191,7 +1212,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1243,7 +1264,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1340,7 +1361,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1401,7 +1422,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1458,7 +1479,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1525,7 +1546,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1668,34 +1689,65 @@
 <file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44993</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>Heartland Express</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>16.260000000000002</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>1283.5806600000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>1763.72066</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>1294.1990734380452</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>16.394510754082734</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="N17">
+            <v>321.39600000000002</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44595</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1704,34 +1756,59 @@
 <file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44993</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>ArcBest Corporation</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>101.62</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="N8">
+            <v>2498.3277000000003</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>2754.4777000000004</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>3083.7037867156318</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>125.4302943549169</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="N17">
+            <v>539.48500000000149</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1747,23 +1824,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1783,23 +1860,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>8.1999999999999993</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>3802.98</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="J18">
-            <v>218.76521315251679</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="J19">
-            <v>2.7483066978959396</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1848,65 +1925,70 @@
 <file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="N2">
-            <v>44993</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="N4" t="str">
-            <v>Heartland Express</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>16.260000000000002</v>
+        <row r="3">
+          <cell r="N3">
+            <v>4.43</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>1283.5806600000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="N11">
-            <v>1763.72066</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>1294.1990734380452</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="N15">
-            <v>16.394510754082734</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="N17">
-            <v>321.39600000000002</v>
+            <v>217.09325999999999</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>42.225188935657137</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>0.9450156424434254</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="J1">
-            <v>44595</v>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>8.1999999999999993</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="J8">
+            <v>3802.98</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="J18">
+            <v>218.76521315251679</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="J19">
+            <v>2.7483066978959396</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2425,11 +2507,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569CADF2-2E0D-4D7A-9853-86DF7D017A5C}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2445,10 +2527,10 @@
     <col min="9" max="9" width="7.5703125" style="13" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5703125" style="19" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="32" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2486,10 +2568,10 @@
       <c r="K1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="31" t="s">
         <v>125</v>
       </c>
       <c r="N1" s="19" t="s">
@@ -2498,7 +2580,7 @@
       <c r="O1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="32" t="s">
         <v>84</v>
       </c>
       <c r="Q1" t="s">
@@ -2515,7 +2597,7 @@
       <c r="C2" s="4">
         <v>44775</v>
       </c>
-      <c r="D2" s="30"/>
+      <c r="D2" s="28"/>
       <c r="E2" t="s">
         <v>73</v>
       </c>
@@ -2541,7 +2623,7 @@
         <f>[1]Main!$N$20</f>
         <v>506.49669636225735</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="32">
         <f>O2/N2</f>
         <v>4.733613984693994</v>
       </c>
@@ -2559,7 +2641,7 @@
       <c r="C3" s="4">
         <v>44772</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="28"/>
       <c r="E3" t="s">
         <v>22</v>
       </c>
@@ -2585,7 +2667,7 @@
         <f>[2]Main!$N$19</f>
         <v>605.54899120857669</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="32">
         <f>O3/N3</f>
         <v>4.3731421333760139</v>
       </c>
@@ -2603,7 +2685,7 @@
       <c r="C4" s="4">
         <v>44773</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="28"/>
       <c r="E4" t="s">
         <v>22</v>
       </c>
@@ -2629,7 +2711,7 @@
         <f>[3]Main!$N$19</f>
         <v>52.989005935204794</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="32">
         <f t="shared" ref="P4:P17" si="0">O4/N4</f>
         <v>1.5006798622261339</v>
       </c>
@@ -2644,7 +2726,7 @@
       <c r="C5" s="4">
         <v>44773</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="28"/>
       <c r="E5" t="s">
         <v>5</v>
       </c>
@@ -2670,7 +2752,7 @@
         <f>[4]Main!$N$20</f>
         <v>66.876035494517382</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="32">
         <f t="shared" si="0"/>
         <v>1.0333132801995888</v>
       </c>
@@ -2685,7 +2767,7 @@
       <c r="C6" s="4">
         <v>44773</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="28"/>
       <c r="E6" t="s">
         <v>22</v>
       </c>
@@ -2711,7 +2793,7 @@
         <f>[5]Main!$N$19</f>
         <v>436.69397285882815</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="32">
         <f t="shared" si="0"/>
         <v>5.0194709524003231</v>
       </c>
@@ -2726,7 +2808,7 @@
       <c r="C7" s="4">
         <v>44774</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="28"/>
       <c r="E7" t="s">
         <v>22</v>
       </c>
@@ -2752,7 +2834,7 @@
         <f>[6]Main!$N$19</f>
         <v>294.64223261975781</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="32">
         <f t="shared" si="0"/>
         <v>4.0109206727437767</v>
       </c>
@@ -2767,7 +2849,7 @@
       <c r="C8" s="4">
         <v>44774</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="28"/>
       <c r="E8" t="s">
         <v>5</v>
       </c>
@@ -2793,7 +2875,7 @@
         <f>[7]Main!$N$19</f>
         <v>142.2079469106753</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="32">
         <f t="shared" si="0"/>
         <v>2.2068272332507033</v>
       </c>
@@ -2808,7 +2890,7 @@
       <c r="C9" s="4">
         <v>44774</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="28"/>
       <c r="E9" t="s">
         <v>22</v>
       </c>
@@ -2834,7 +2916,7 @@
         <f>[8]Main!$N$19</f>
         <v>49.564500982059428</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="32">
         <f t="shared" si="0"/>
         <v>1.9684075052446159</v>
       </c>
@@ -2849,7 +2931,7 @@
       <c r="C10" s="4">
         <v>44775</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="28"/>
       <c r="E10" t="s">
         <v>22</v>
       </c>
@@ -2875,7 +2957,7 @@
         <f>[9]Main!$N$19</f>
         <v>357.06180902658434</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="32">
         <f t="shared" si="0"/>
         <v>1.3716264944168115</v>
       </c>
@@ -2890,7 +2972,7 @@
       <c r="C11" s="4">
         <v>44775</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="28"/>
       <c r="E11" t="s">
         <v>22</v>
       </c>
@@ -2916,7 +2998,7 @@
         <f>[10]Main!$N$19</f>
         <v>86.349119613796859</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="32">
         <f>O11/N11</f>
         <v>1.4218527846829716</v>
       </c>
@@ -2931,7 +3013,7 @@
       <c r="C12" s="4">
         <v>44775</v>
       </c>
-      <c r="D12" s="30"/>
+      <c r="D12" s="28"/>
       <c r="E12" t="s">
         <v>22</v>
       </c>
@@ -2957,7 +3039,7 @@
         <f>[11]Main!$N$19</f>
         <v>17.243419112262924</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="32">
         <f t="shared" si="0"/>
         <v>0.82662603606246043</v>
       </c>
@@ -2976,7 +3058,7 @@
       <c r="C13" s="4">
         <v>44984</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>44951</v>
       </c>
       <c r="E13" t="s">
@@ -3004,12 +3086,12 @@
         <f>+SUM([12]Model!$L$15:$O$15)</f>
         <v>7318.0999999999985</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="30">
         <f t="shared" ref="L13:L26" si="1">K13/(J13/O13)</f>
         <v>21.261185357350374</v>
       </c>
-      <c r="M13" s="28">
-        <f t="shared" ref="M13:M26" si="2">H13/K13</f>
+      <c r="M13" s="31">
+        <f t="shared" ref="M13:M25" si="2">H13/K13</f>
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
@@ -3020,7 +3102,7 @@
         <f>+[12]Main!$N$14</f>
         <v>163.0331173825</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="32">
         <f t="shared" si="0"/>
         <v>1.7819774552683354</v>
       </c>
@@ -3035,7 +3117,7 @@
       <c r="C14" s="4">
         <v>44973</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>44964</v>
       </c>
       <c r="E14" t="s">
@@ -3063,11 +3145,11 @@
         <f>+[13]Model!$AA$27</f>
         <v>642.59899999999948</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="30">
         <f t="shared" si="1"/>
         <v>2.519294627770305</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="31">
         <f t="shared" si="2"/>
         <v>65.181544400162522</v>
       </c>
@@ -3079,7 +3161,7 @@
         <f>[13]Main!$N$13</f>
         <v>69.464871001991241</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="32">
         <f t="shared" si="0"/>
         <v>0.91702800002628704</v>
       </c>
@@ -3094,7 +3176,7 @@
       <c r="C15" s="4">
         <v>44972</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>44916</v>
       </c>
       <c r="E15" t="s">
@@ -3122,11 +3204,11 @@
         <f>+[14]Model!$Z$27</f>
         <v>-2103</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="30">
         <f t="shared" si="1"/>
         <v>-1.7809748892171344</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15" s="31">
         <f t="shared" si="2"/>
         <v>-20.909710933439491</v>
       </c>
@@ -3138,7 +3220,7 @@
         <f>[14]Main!$N$13</f>
         <v>15.962243022133215</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="32">
         <f t="shared" si="0"/>
         <v>1.3094538984522737</v>
       </c>
@@ -3154,7 +3236,7 @@
         <f>+[15]Main!$N$2</f>
         <v>44985</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <v>44985</v>
       </c>
       <c r="E16" t="s">
@@ -3182,11 +3264,11 @@
         <f>+SUM([15]Model!$G$26:$J$26)</f>
         <v>-802.42000000000019</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="30">
         <f t="shared" si="1"/>
         <v>-2.1957099349019975</v>
       </c>
-      <c r="M16" s="28">
+      <c r="M16" s="31">
         <f t="shared" si="2"/>
         <v>-22.711573041549308</v>
       </c>
@@ -3198,12 +3280,12 @@
         <f>[15]Main!$N$13</f>
         <v>26.170829625152908</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="32">
         <f t="shared" si="0"/>
         <v>1.7974470896396229</v>
       </c>
     </row>
-    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -3213,7 +3295,7 @@
       <c r="C17" s="4">
         <v>44972</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>44867</v>
       </c>
       <c r="E17" t="s">
@@ -3240,11 +3322,11 @@
       <c r="K17" s="13">
         <v>2</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="30">
         <f t="shared" si="1"/>
         <v>3.7703836365350178E-2</v>
       </c>
-      <c r="M17" s="28">
+      <c r="M17" s="31">
         <f t="shared" si="2"/>
         <v>544.56130000000007</v>
       </c>
@@ -3256,12 +3338,12 @@
         <f>[16]Main!$N$13</f>
         <v>8.932840074054166</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17" s="32">
         <f t="shared" si="0"/>
         <v>0.76479795154573338</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -3271,7 +3353,7 @@
       <c r="C18" s="4">
         <v>44979</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="28">
         <v>44950</v>
       </c>
       <c r="E18" t="s">
@@ -3299,11 +3381,11 @@
         <f>[17]Model!$X$28</f>
         <v>11119</v>
       </c>
-      <c r="L18" s="29">
+      <c r="L18" s="30">
         <f t="shared" si="1"/>
         <v>12.138646288209607</v>
       </c>
-      <c r="M18" s="28">
+      <c r="M18" s="31">
         <f t="shared" si="2"/>
         <v>14.035057109452291</v>
       </c>
@@ -3315,15 +3397,15 @@
         <f>[17]Main!$N$13</f>
         <v>146.82271084967829</v>
       </c>
-      <c r="P18" s="14">
-        <f t="shared" ref="P18:P27" si="3">O18/N18</f>
+      <c r="P18" s="32">
+        <f t="shared" ref="P18:P28" si="3">O18/N18</f>
         <v>0.86468027591094387</v>
       </c>
       <c r="Q18" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -3333,7 +3415,7 @@
       <c r="C19" s="4">
         <v>44980</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="28">
         <v>44972</v>
       </c>
       <c r="E19" t="s">
@@ -3361,11 +3443,11 @@
         <f>SUM([18]Model!$J$29:$M$29)</f>
         <v>1530.8109999999983</v>
       </c>
-      <c r="L19" s="29">
+      <c r="L19" s="30">
         <f t="shared" si="1"/>
         <v>3.0186366146079791</v>
       </c>
-      <c r="M19" s="28">
+      <c r="M19" s="31">
         <f t="shared" si="2"/>
         <v>65.034042739436885</v>
       </c>
@@ -3377,7 +3459,7 @@
         <f>+[18]Main!$N$14</f>
         <v>188.40829140695323</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="32">
         <f t="shared" si="3"/>
         <v>1.0148574813194355</v>
       </c>
@@ -3385,7 +3467,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -3395,7 +3477,7 @@
       <c r="C20" s="4">
         <v>44981</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>44963</v>
       </c>
       <c r="E20" t="s">
@@ -3423,11 +3505,11 @@
         <f>+[19]Model!$X$29</f>
         <v>2922.8000000000011</v>
       </c>
-      <c r="L20" s="29">
+      <c r="L20" s="30">
         <f t="shared" si="1"/>
         <v>6.7469990766389687</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20" s="31">
         <f t="shared" si="2"/>
         <v>11.691219378677975</v>
       </c>
@@ -3439,7 +3521,7 @@
         <f>+[19]Main!$N$16</f>
         <v>81.049559034736063</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="32">
         <f t="shared" si="3"/>
         <v>1.0625269931140018</v>
       </c>
@@ -3447,7 +3529,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -3457,7 +3539,7 @@
       <c r="C21" s="4">
         <v>44982</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="28">
         <v>44959</v>
       </c>
       <c r="E21" t="s">
@@ -3485,11 +3567,11 @@
         <f>+SUM([20]Model!$F$28:$I$28)</f>
         <v>3890.6999999999989</v>
       </c>
-      <c r="L21" s="29">
+      <c r="L21" s="30">
         <f t="shared" si="1"/>
         <v>7.0843044428259256</v>
       </c>
-      <c r="M21" s="28">
+      <c r="M21" s="31">
         <f t="shared" si="2"/>
         <v>12.866593672089859</v>
       </c>
@@ -3501,7 +3583,7 @@
         <f>+[20]Main!$N$15</f>
         <v>89.941774978464281</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="32">
         <f t="shared" si="3"/>
         <v>1.1287873365771119</v>
       </c>
@@ -3509,7 +3591,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -3519,7 +3601,7 @@
       <c r="C22" s="4">
         <v>44983</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="28">
         <v>44895</v>
       </c>
       <c r="E22" t="s">
@@ -3547,11 +3629,11 @@
         <f>SUM([21]Model!$F$28:$I$28)</f>
         <v>226.52699999999987</v>
       </c>
-      <c r="L22" s="29">
+      <c r="L22" s="30">
         <f t="shared" si="1"/>
         <v>3.5525845304560546</v>
       </c>
-      <c r="M22" s="28">
+      <c r="M22" s="31">
         <f t="shared" si="2"/>
         <v>8.0717101272696024</v>
       </c>
@@ -3563,7 +3645,7 @@
         <f>+[21]Main!$N$15</f>
         <v>34.090495572360147</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22" s="32">
         <f t="shared" si="3"/>
         <v>1.1169887146906994</v>
       </c>
@@ -3571,7 +3653,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -3581,7 +3663,7 @@
       <c r="C23" s="4">
         <v>44991</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="28">
         <v>44958</v>
       </c>
       <c r="E23" t="s">
@@ -3610,11 +3692,11 @@
         <f>+[22]Model!$T$32</f>
         <v>2116.6350000000002</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="30">
         <f t="shared" si="1"/>
         <v>18.841329891401102</v>
       </c>
-      <c r="M23" s="28">
+      <c r="M23" s="31">
         <f t="shared" si="2"/>
         <v>18.718866502727206</v>
       </c>
@@ -3626,7 +3708,7 @@
         <f>+[22]Main!$N$15</f>
         <v>305.59480206667075</v>
       </c>
-      <c r="P23" s="14">
+      <c r="P23" s="32">
         <f t="shared" si="3"/>
         <v>0.8658302934315647</v>
       </c>
@@ -3634,7 +3716,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -3645,7 +3727,7 @@
         <f>+[23]Main!$N$2</f>
         <v>44992</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="28">
         <f>+[23]Model!$J$1</f>
         <v>44595</v>
       </c>
@@ -3675,11 +3757,11 @@
         <f>+[23]Model!$T$28</f>
         <v>627.74999999999977</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="30">
         <f t="shared" si="1"/>
         <v>23.670814479638004</v>
       </c>
-      <c r="M24" s="28">
+      <c r="M24" s="31">
         <f t="shared" si="2"/>
         <v>12.278009398645962</v>
       </c>
@@ -3691,7 +3773,7 @@
         <f>+[23]Main!$N$15</f>
         <v>289.77104778090956</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24" s="32">
         <f t="shared" si="3"/>
         <v>1.0034665920314076</v>
       </c>
@@ -3699,7 +3781,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -3710,7 +3792,7 @@
         <f>+[24]Main!$N$2</f>
         <v>44992</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="28">
         <f>+[24]Model!$J$1</f>
         <v>44605</v>
       </c>
@@ -3740,11 +3822,11 @@
         <f>+[24]Model!$T$31</f>
         <v>186.68</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="30">
         <f t="shared" si="1"/>
         <v>8.320556248885719</v>
       </c>
-      <c r="M25" s="28">
+      <c r="M25" s="31">
         <f t="shared" si="2"/>
         <v>4.571692950503536</v>
       </c>
@@ -3756,15 +3838,15 @@
         <f>+[24]Main!$N$15</f>
         <v>43.274386114774124</v>
       </c>
-      <c r="P25" s="14">
+      <c r="P25" s="32">
         <f t="shared" si="3"/>
         <v>1.4799721653479523</v>
       </c>
-      <c r="Q25" s="31" t="s">
+      <c r="Q25" s="29" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -3775,7 +3857,7 @@
         <f>+[25]Main!$N$2</f>
         <v>44992</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="28">
         <f>+[25]Model!$J$1</f>
         <v>44951</v>
       </c>
@@ -3805,11 +3887,11 @@
         <f>+[25]Model!$T$35</f>
         <v>178.19999999999982</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="30">
         <f t="shared" si="1"/>
         <v>11.875249900039972</v>
       </c>
-      <c r="M26" s="28">
+      <c r="M26" s="31">
         <f>H26/K26</f>
         <v>3.5680259259259288</v>
       </c>
@@ -3821,7 +3903,7 @@
         <f>+[25]Main!$N$15</f>
         <v>44.985729196164556</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="32">
         <f t="shared" si="3"/>
         <v>1.2718611590660038</v>
       </c>
@@ -3829,7 +3911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -3837,11 +3919,11 @@
         <v>141</v>
       </c>
       <c r="C27" s="4">
-        <f>+[30]Main!$N$2</f>
+        <f>+[26]Main!$N$2</f>
         <v>44993</v>
       </c>
-      <c r="D27" s="30">
-        <f>+[30]Model!$J$1</f>
+      <c r="D27" s="28">
+        <f>+[26]Model!$J$1</f>
         <v>44595</v>
       </c>
       <c r="E27" t="s">
@@ -3851,53 +3933,117 @@
         <v>150</v>
       </c>
       <c r="G27" t="str">
-        <f>+[30]Main!$N$4</f>
+        <f>+[26]Main!$N$4</f>
         <v>Heartland Express</v>
       </c>
       <c r="H27" s="12">
-        <f>+[30]Main!$N$11</f>
+        <f>+[26]Main!$N$11</f>
         <v>1763.72066</v>
       </c>
       <c r="I27" s="13">
-        <f>+[30]Main!$N$8</f>
+        <f>+[26]Main!$N$8</f>
         <v>1283.5806600000001</v>
       </c>
       <c r="J27" s="13">
-        <f>+[30]Main!$N$14</f>
+        <f>+[26]Main!$N$14</f>
         <v>1294.1990734380452</v>
       </c>
       <c r="K27" s="13">
-        <f>+[30]Main!$N$17</f>
+        <f>+[26]Main!$N$17</f>
         <v>321.39600000000002</v>
       </c>
-      <c r="L27" s="29">
-        <f t="shared" ref="L27" si="4">K27/(J27/O27)</f>
+      <c r="L27" s="30">
+        <f t="shared" ref="L27:L28" si="4">K27/(J27/O27)</f>
         <v>4.0713444217833574</v>
       </c>
-      <c r="M27" s="28">
+      <c r="M27" s="31">
         <f>H27/K27</f>
         <v>5.4876870278410435</v>
       </c>
       <c r="N27" s="19">
-        <f>+[30]Main!$N$6</f>
+        <f>+[26]Main!$N$6</f>
         <v>16.260000000000002</v>
       </c>
       <c r="O27" s="19">
-        <f>+[30]Main!$N$15</f>
+        <f>+[26]Main!$N$15</f>
         <v>16.394510754082734</v>
       </c>
-      <c r="P27" s="14">
+      <c r="P27" s="32">
         <f t="shared" si="3"/>
         <v>1.008272494101029</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>140</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>141</v>
       </c>
+      <c r="C28" s="4">
+        <f>+[27]Main!$N$2</f>
+        <v>44993</v>
+      </c>
+      <c r="D28" s="28">
+        <f>+[27]Model!$J$1</f>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" t="str">
+        <f>+[27]Main!$N$4</f>
+        <v>ArcBest Corporation</v>
+      </c>
+      <c r="H28" s="12">
+        <f>+[27]Main!$N$11</f>
+        <v>2754.4777000000004</v>
+      </c>
+      <c r="I28" s="13">
+        <f>+[27]Main!$N$8</f>
+        <v>2498.3277000000003</v>
+      </c>
+      <c r="J28" s="13">
+        <f>+[27]Main!$N$14</f>
+        <v>3083.7037867156318</v>
+      </c>
+      <c r="K28" s="13">
+        <f>+[27]Main!$N$17</f>
+        <v>539.48500000000149</v>
+      </c>
+      <c r="L28" s="30">
+        <f t="shared" si="4"/>
+        <v>21.943664836282345</v>
+      </c>
+      <c r="M28" s="31">
+        <f>H28/K28</f>
+        <v>5.1057540061354674</v>
+      </c>
+      <c r="N28" s="19">
+        <f>+[27]Main!$N$6</f>
+        <v>101.62</v>
+      </c>
+      <c r="O28" s="19">
+        <f>+[27]Main!$N$15</f>
+        <v>125.4302943549169</v>
+      </c>
+      <c r="P28" s="32">
+        <f t="shared" si="3"/>
+        <v>1.2343071674366946</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P1:P1048576">
@@ -3939,9 +4085,10 @@
     <hyperlink ref="F25" r:id="rId24" xr:uid="{B7CF3F61-BFC6-41D5-8919-5EDA0850C31F}"/>
     <hyperlink ref="F26" r:id="rId25" xr:uid="{2F373320-D823-4882-B676-2DA2483444D3}"/>
     <hyperlink ref="F27" r:id="rId26" xr:uid="{3EE9ACF3-C9F0-41B1-A950-5743DB0F0BEE}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{3B7812D1-B655-48B8-B61A-D17304EE6F0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -4316,19 +4463,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[26]Main!$J$8</f>
+        <f>+[28]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[26]Main!$J$18</f>
+        <f>+[28]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[26]Main!$J$3</f>
+        <f>+[28]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[26]Main!$J$19</f>
+        <f>+[28]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -4611,19 +4758,19 @@
         <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[27]Main!$O$8</f>
+        <f>[29]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[27]Main!$O$18</f>
+        <f>[29]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[27]Main!$O$3</f>
+        <f>[29]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[27]Main!$O$19</f>
+        <f>[29]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -4651,19 +4798,19 @@
         <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[28]Main!$N$8</f>
+        <f>+[30]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[28]Main!$N$18</f>
+        <f>+[30]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[28]Main!$N$3</f>
+        <f>+[30]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[28]Main!$N$19</f>
+        <f>+[30]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -4694,19 +4841,19 @@
         <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[29]Main!$J$8</f>
+        <f>[31]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[29]Main!$J$18</f>
+        <f>[31]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[29]Main!$J$3</f>
+        <f>[31]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[29]Main!$J$19</f>
+        <f>[31]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">

</xml_diff>

<commit_message>
2023Q1 Update for Covenant Logistics Group (CVLG)
Company is now perfectly valued, will be scaling out of my position.

Price target 22Q4: $44.99
Price target 23Q1: $40.91
</commit_message>
<xml_diff>
--- a/DCF Portfolio.xlsx
+++ b/DCF Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\Main\investingModels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B27EA-7E80-4BDB-BF06-DCDF4F809521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE25EE82-04FB-4C5E-85D1-C7404495CE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="6210" windowWidth="30720" windowHeight="15045" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
+    <workbookView xWindow="21240" yWindow="6060" windowWidth="19290" windowHeight="14820" xr2:uid="{3E88963E-B2BB-4D5E-8FAE-1DA3A47B0DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="WatchList" sheetId="1" r:id="rId1"/>
@@ -50,6 +50,7 @@
     <externalReference r:id="rId33"/>
     <externalReference r:id="rId34"/>
     <externalReference r:id="rId35"/>
+    <externalReference r:id="rId36"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -767,22 +768,7 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>60.73</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>5961.5730000000003</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="N18">
-            <v>6053.073284927159</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="N19">
-            <v>86.349119613796859</v>
+            <v>207.35</v>
           </cell>
         </row>
       </sheetData>
@@ -803,22 +789,22 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>20.86</v>
+            <v>60.73</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>3705.70046</v>
+            <v>5961.5730000000003</v>
           </cell>
         </row>
         <row r="18">
           <cell r="N18">
-            <v>2666.8844433216959</v>
+            <v>6053.073284927159</v>
           </cell>
         </row>
         <row r="19">
           <cell r="N19">
-            <v>17.243419112262924</v>
+            <v>86.349119613796859</v>
           </cell>
         </row>
       </sheetData>
@@ -831,59 +817,34 @@
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="5">
-          <cell r="N5">
-            <v>91.49</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="N7">
-            <v>31490.857999999997</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="N10">
-            <v>34568.657999999996</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="N13">
-            <v>56115.999003056495</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>163.0331173825</v>
+        <row r="3">
+          <cell r="N3">
+            <v>20.86</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>3705.70046</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>2666.8844433216959</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>17.243419112262924</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="15">
-          <cell r="L15">
-            <v>1874.0000000000005</v>
-          </cell>
-          <cell r="M15">
-            <v>2168.1</v>
-          </cell>
-          <cell r="N15">
-            <v>2046.4999999999977</v>
-          </cell>
-          <cell r="O15">
-            <v>1229.5</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -902,40 +863,49 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="4">
-          <cell r="N4">
-            <v>75.75</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>19321.628250000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="N9">
-            <v>41885.595249999998</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="N12">
-            <v>17718.474111348907</v>
+        <row r="5">
+          <cell r="N5">
+            <v>91.49</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="N7">
+            <v>31490.857999999997</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>34568.657999999996</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>69.464871001991241</v>
+            <v>56115.999003056495</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>163.0331173825</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="27">
-          <cell r="AA27">
-            <v>642.59899999999948</v>
+        <row r="15">
+          <cell r="L15">
+            <v>1874.0000000000005</v>
+          </cell>
+          <cell r="M15">
+            <v>2168.1</v>
+          </cell>
+          <cell r="N15">
+            <v>2046.4999999999977</v>
+          </cell>
+          <cell r="O15">
+            <v>1229.5</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -956,38 +926,38 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="N4">
-            <v>12.19</v>
+            <v>75.75</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>14394.122093023256</v>
+            <v>19321.628250000002</v>
           </cell>
         </row>
         <row r="9">
           <cell r="N9">
-            <v>43973.122093023252</v>
+            <v>41885.595249999998</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>18848.439289507303</v>
+            <v>17718.474111348907</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>15.962243022133215</v>
+            <v>69.464871001991241</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="27">
-          <cell r="Z27">
-            <v>-2103</v>
+          <cell r="AA27">
+            <v>642.59899999999948</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1006,54 +976,40 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="N2">
-            <v>44985</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="N4">
-            <v>14.56</v>
+            <v>12.19</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>5320.9374400000006</v>
+            <v>14394.122093023256</v>
           </cell>
         </row>
         <row r="9">
           <cell r="N9">
-            <v>18224.220440000001</v>
+            <v>43973.122093023252</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>9564.1035156825055</v>
+            <v>18848.439289507303</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>26.170829625152908</v>
+            <v>15.962243022133215</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="26">
-          <cell r="G26">
-            <v>-509.65600000000006</v>
-          </cell>
-          <cell r="H26">
-            <v>-215.28849999999991</v>
-          </cell>
-          <cell r="I26">
-            <v>1.2999999999998977</v>
-          </cell>
-          <cell r="J26">
-            <v>-78.775500000000051</v>
+        <row r="27">
+          <cell r="Z27">
+            <v>-2103</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1072,34 +1028,54 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="2">
+          <cell r="N2">
+            <v>44985</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="N4">
-            <v>11.68</v>
+            <v>14.56</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>619.56560000000002</v>
+            <v>5320.9374400000006</v>
           </cell>
         </row>
         <row r="9">
           <cell r="N9">
-            <v>1089.1226000000001</v>
+            <v>18224.220440000001</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>473.84250172820322</v>
+            <v>9564.1035156825055</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>8.932840074054166</v>
+            <v>26.170829625152908</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="26">
+          <cell r="G26">
+            <v>-509.65600000000006</v>
+          </cell>
+          <cell r="H26">
+            <v>-215.28849999999991</v>
+          </cell>
+          <cell r="I26">
+            <v>1.2999999999998977</v>
+          </cell>
+          <cell r="J26">
+            <v>-78.775500000000051</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1118,40 +1094,34 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="5">
-          <cell r="N5">
-            <v>169.8</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="N7">
-            <v>155536.80000000002</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="N10">
-            <v>156055.80000000002</v>
+        <row r="4">
+          <cell r="N4">
+            <v>11.68</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>619.56560000000002</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="N9">
+            <v>1089.1226000000001</v>
           </cell>
         </row>
         <row r="12">
           <cell r="N12">
-            <v>134489.60313830531</v>
+            <v>473.84250172820322</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>146.82271084967829</v>
+            <v>8.932840074054166</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="28">
-          <cell r="X28">
-            <v>11119</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1172,47 +1142,38 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="N5">
-            <v>185.65</v>
+            <v>169.8</v>
           </cell>
         </row>
         <row r="7">
           <cell r="N7">
-            <v>94146.828000000009</v>
+            <v>155536.80000000002</v>
           </cell>
         </row>
         <row r="10">
           <cell r="N10">
-            <v>99554.828000000009</v>
+            <v>156055.80000000002</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>134489.60313830531</v>
           </cell>
         </row>
         <row r="13">
           <cell r="N13">
-            <v>95545.612738294119</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>188.40829140695323</v>
+            <v>146.82271084967829</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="29">
-          <cell r="J29">
-            <v>303.0739999999995</v>
-          </cell>
-          <cell r="K29">
-            <v>268.88500000000033</v>
-          </cell>
-          <cell r="L29">
-            <v>472.50999999999863</v>
-          </cell>
-          <cell r="M29">
-            <v>486.34199999999987</v>
+        <row r="28">
+          <cell r="X28">
+            <v>11119</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1231,40 +1192,49 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="5">
+          <cell r="N5">
+            <v>185.65</v>
+          </cell>
+        </row>
         <row r="7">
           <cell r="N7">
-            <v>76.28</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="N9">
-            <v>33044.495999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="N12">
-            <v>34171.095999999998</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="N15">
-            <v>35110.668973847663</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="N16">
-            <v>81.049559034736063</v>
+            <v>94146.828000000009</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="N10">
+            <v>99554.828000000009</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="N13">
+            <v>95545.612738294119</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>188.40829140695323</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="29">
-          <cell r="X29">
-            <v>2922.8000000000011</v>
+          <cell r="J29">
+            <v>303.0739999999995</v>
+          </cell>
+          <cell r="K29">
+            <v>268.88500000000033</v>
+          </cell>
+          <cell r="L29">
+            <v>472.50999999999863</v>
+          </cell>
+          <cell r="M29">
+            <v>486.34199999999987</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1319,49 +1289,40 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="6">
-          <cell r="N6">
-            <v>79.680000000000007</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="N8">
-            <v>43760.256000000008</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="N11">
-            <v>50060.056000000004</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>49396.022818172591</v>
+        <row r="7">
+          <cell r="N7">
+            <v>76.28</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="N9">
+            <v>33044.495999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="N12">
+            <v>34171.095999999998</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>89.941774978464281</v>
+            <v>35110.668973847663</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="N16">
+            <v>81.049559034736063</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="28">
-          <cell r="F28">
-            <v>854.99999999999932</v>
-          </cell>
-          <cell r="G28">
-            <v>964.69999999999982</v>
-          </cell>
-          <cell r="H28">
-            <v>1011.1999999999999</v>
-          </cell>
-          <cell r="I28">
-            <v>1059.7999999999997</v>
+        <row r="29">
+          <cell r="X29">
+            <v>2922.8000000000011</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1382,47 +1343,47 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="N6">
-            <v>30.52</v>
+            <v>79.680000000000007</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>1946.07728</v>
+            <v>43760.256000000008</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>1828.46028</v>
+            <v>50060.056000000004</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>2173.7463596759726</v>
+            <v>49396.022818172591</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>34.090495572360147</v>
+            <v>89.941774978464281</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="28">
           <cell r="F28">
-            <v>52.289999999999864</v>
+            <v>854.99999999999932</v>
           </cell>
           <cell r="G28">
-            <v>55.844000000000015</v>
+            <v>964.69999999999982</v>
           </cell>
           <cell r="H28">
-            <v>72.525999999999996</v>
+            <v>1011.1999999999999</v>
           </cell>
           <cell r="I28">
-            <v>45.867000000000004</v>
+            <v>1059.7999999999997</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1441,45 +1402,49 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="4">
-          <cell r="N4" t="str">
-            <v>Old Dominion Freight Line</v>
-          </cell>
-        </row>
         <row r="6">
           <cell r="N6">
-            <v>352.95</v>
+            <v>30.52</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>39650.402999999998</v>
+            <v>1946.07728</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>39621.008000000002</v>
+            <v>1828.46028</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>34330.520064169796</v>
+            <v>2173.7463596759726</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>305.59480206667075</v>
+            <v>34.090495572360147</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="32">
-          <cell r="T32">
-            <v>2116.6350000000002</v>
+        <row r="28">
+          <cell r="F28">
+            <v>52.289999999999864</v>
+          </cell>
+          <cell r="G28">
+            <v>55.844000000000015</v>
+          </cell>
+          <cell r="H28">
+            <v>72.525999999999996</v>
+          </cell>
+          <cell r="I28">
+            <v>45.867000000000004</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1498,55 +1463,45 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="N2">
-            <v>44992</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>Saia</v>
+            <v>Old Dominion Freight Line</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>288.77</v>
+            <v>352.95</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>7658.1803999999993</v>
+            <v>39650.402999999998</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>7707.5203999999994</v>
+            <v>39621.008000000002</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>7684.7281871497207</v>
+            <v>34330.520064169796</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>289.77104778090956</v>
+            <v>305.59480206667075</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="1">
-          <cell r="J1">
-            <v>44595</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="T28">
-            <v>627.74999999999977</v>
+        <row r="32">
+          <cell r="T32">
+            <v>2116.6350000000002</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1572,48 +1527,48 @@
         </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>P.A.M. Transportation Services</v>
+            <v>Saia</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>29.24</v>
+            <v>288.77</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>656.02864</v>
+            <v>7658.1803999999993</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>853.44364000000007</v>
+            <v>7707.5203999999994</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>970.90412687107221</v>
+            <v>7684.7281871497207</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>43.274386114774124</v>
+            <v>289.77104778090956</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="J1">
-            <v>44605</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="T31">
-            <v>186.68</v>
+            <v>44595</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="T28">
+            <v>627.74999999999977</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1639,48 +1594,48 @@
         </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>Covenant Logistics Group</v>
+            <v>P.A.M. Transportation Services</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>35.369999999999997</v>
+            <v>29.24</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>530.76221999999996</v>
+            <v>656.02864</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>635.8222199999999</v>
+            <v>853.44364000000007</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>675.0558523176453</v>
+            <v>970.90412687107221</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>44.985729196164556</v>
+            <v>43.274386114774124</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="J1">
-            <v>44951</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="T35">
-            <v>178.19999999999982</v>
+            <v>44605</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="T31">
+            <v>186.68</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1701,53 +1656,53 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="N2">
-            <v>44993</v>
+            <v>45047</v>
           </cell>
         </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>Heartland Express</v>
+            <v>Covenant Logistics Group</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>16.260000000000002</v>
+            <v>42.18</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>1283.5806600000001</v>
+            <v>563.56698000000006</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>1763.72066</v>
+            <v>628.53698000000009</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>1294.1990734380452</v>
+            <v>546.57156432801094</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>16.394510754082734</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="N17">
-            <v>321.39600000000002</v>
+            <v>40.907983259337691</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="1">
-          <cell r="J1">
-            <v>44595</v>
+          <cell r="K1">
+            <v>45044</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="U35">
+            <v>178.19999999999982</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1773,42 +1728,48 @@
         </row>
         <row r="4">
           <cell r="N4" t="str">
-            <v>ArcBest Corporation</v>
+            <v>Heartland Express</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>101.62</v>
+            <v>16.260000000000002</v>
           </cell>
         </row>
         <row r="8">
           <cell r="N8">
-            <v>2498.3277000000003</v>
+            <v>1283.5806600000001</v>
           </cell>
         </row>
         <row r="11">
           <cell r="N11">
-            <v>2754.4777000000004</v>
+            <v>1763.72066</v>
           </cell>
         </row>
         <row r="14">
           <cell r="N14">
-            <v>3083.7037867156318</v>
+            <v>1294.1990734380452</v>
           </cell>
         </row>
         <row r="15">
           <cell r="N15">
-            <v>125.4302943549169</v>
+            <v>16.394510754082734</v>
           </cell>
         </row>
         <row r="17">
           <cell r="N17">
-            <v>539.48500000000149</v>
+            <v>321.39600000000002</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="J1">
+            <v>44595</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1817,34 +1778,59 @@
 <file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Dash"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>67.2</v>
+        <row r="2">
+          <cell r="N2">
+            <v>44993</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="N4" t="str">
+            <v>ArcBest Corporation</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>101.62</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="J8">
-            <v>87517.207200000004</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="J18">
-            <v>74903.518611460153</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="J19">
-            <v>63.631730278242067</v>
+          <cell r="N8">
+            <v>2498.3277000000003</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="N11">
+            <v>2754.4777000000004</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="N14">
+            <v>3083.7037867156318</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="N15">
+            <v>125.4302943549169</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="N17">
+            <v>539.48500000000149</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1860,23 +1846,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="O3">
-            <v>18.149999999999999</v>
+          <cell r="J3">
+            <v>67.2</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="O8">
-            <v>506.71814999999992</v>
+          <cell r="J8">
+            <v>87517.207200000004</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="O18">
-            <v>541.46267091390234</v>
+          <cell r="J18">
+            <v>74903.518611460153</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="O19">
-            <v>16.629178185986376</v>
+          <cell r="J19">
+            <v>63.631730278242067</v>
           </cell>
         </row>
       </sheetData>
@@ -1932,23 +1918,23 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>4.43</v>
+          <cell r="O3">
+            <v>18.149999999999999</v>
           </cell>
         </row>
         <row r="8">
-          <cell r="N8">
-            <v>217.09325999999999</v>
+          <cell r="O8">
+            <v>506.71814999999992</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="N18">
-            <v>42.225188935657137</v>
+          <cell r="O18">
+            <v>541.46267091390234</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="N19">
-            <v>0.9450156424434254</v>
+          <cell r="O19">
+            <v>16.629178185986376</v>
           </cell>
         </row>
       </sheetData>
@@ -1959,6 +1945,42 @@
 </file>
 
 <file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>4.43</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="N8">
+            <v>217.09325999999999</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="N18">
+            <v>42.225188935657137</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="N19">
+            <v>0.9450156424434254</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2511,7 +2533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2950,8 +2972,8 @@
         <v>8831.5667844635373</v>
       </c>
       <c r="N10" s="19">
-        <f>[9]Main!$N$3</f>
-        <v>260.32</v>
+        <f>[10]Main!$N$3</f>
+        <v>207.35</v>
       </c>
       <c r="O10" s="19">
         <f>[9]Main!$N$19</f>
@@ -2959,7 +2981,7 @@
       </c>
       <c r="P10" s="32">
         <f t="shared" si="0"/>
-        <v>1.3716264944168115</v>
+        <v>1.7220246396266425</v>
       </c>
     </row>
     <row r="11" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2983,19 +3005,19 @@
         <v>70</v>
       </c>
       <c r="H11" s="12">
-        <f>[10]Main!$N$8</f>
+        <f>[11]Main!$N$8</f>
         <v>5961.5730000000003</v>
       </c>
       <c r="J11" s="13">
-        <f>[10]Main!$N$18</f>
+        <f>[11]Main!$N$18</f>
         <v>6053.073284927159</v>
       </c>
       <c r="N11" s="19">
-        <f>[10]Main!$N$3</f>
+        <f>[11]Main!$N$3</f>
         <v>60.73</v>
       </c>
       <c r="O11" s="19">
-        <f>[10]Main!$N$19</f>
+        <f>[11]Main!$N$19</f>
         <v>86.349119613796859</v>
       </c>
       <c r="P11" s="32">
@@ -3024,19 +3046,19 @@
         <v>75</v>
       </c>
       <c r="H12" s="12">
-        <f>[11]Main!$N$8</f>
+        <f>[12]Main!$N$8</f>
         <v>3705.70046</v>
       </c>
       <c r="J12" s="13">
-        <f>[11]Main!$N$18</f>
+        <f>[12]Main!$N$18</f>
         <v>2666.8844433216959</v>
       </c>
       <c r="N12" s="19">
-        <f>[11]Main!$N$3</f>
+        <f>[12]Main!$N$3</f>
         <v>20.86</v>
       </c>
       <c r="O12" s="19">
-        <f>[11]Main!$N$19</f>
+        <f>[12]Main!$N$19</f>
         <v>17.243419112262924</v>
       </c>
       <c r="P12" s="32">
@@ -3071,19 +3093,19 @@
         <v>96</v>
       </c>
       <c r="H13" s="12">
-        <f>[12]Main!$N$10</f>
+        <f>[13]Main!$N$10</f>
         <v>34568.657999999996</v>
       </c>
       <c r="I13" s="13">
-        <f>+[12]Main!$N$7</f>
+        <f>+[13]Main!$N$7</f>
         <v>31490.857999999997</v>
       </c>
       <c r="J13" s="13">
-        <f>+[12]Main!$N$13</f>
+        <f>+[13]Main!$N$13</f>
         <v>56115.999003056495</v>
       </c>
       <c r="K13" s="13">
-        <f>+SUM([12]Model!$L$15:$O$15)</f>
+        <f>+SUM([13]Model!$L$15:$O$15)</f>
         <v>7318.0999999999985</v>
       </c>
       <c r="L13" s="30">
@@ -3095,11 +3117,11 @@
         <v>4.723720364575505</v>
       </c>
       <c r="N13" s="19">
-        <f>[12]Main!$N$5</f>
+        <f>[13]Main!$N$5</f>
         <v>91.49</v>
       </c>
       <c r="O13" s="19">
-        <f>+[12]Main!$N$14</f>
+        <f>+[13]Main!$N$14</f>
         <v>163.0331173825</v>
       </c>
       <c r="P13" s="32">
@@ -3130,19 +3152,19 @@
         <v>116</v>
       </c>
       <c r="H14" s="12">
-        <f>[13]Main!$N$9</f>
+        <f>[14]Main!$N$9</f>
         <v>41885.595249999998</v>
       </c>
       <c r="I14" s="13">
-        <f>+[13]Main!$N$6</f>
+        <f>+[14]Main!$N$6</f>
         <v>19321.628250000002</v>
       </c>
       <c r="J14" s="13">
-        <f>[13]Main!$N$12</f>
+        <f>[14]Main!$N$12</f>
         <v>17718.474111348907</v>
       </c>
       <c r="K14" s="13">
-        <f>+[13]Model!$AA$27</f>
+        <f>+[14]Model!$AA$27</f>
         <v>642.59899999999948</v>
       </c>
       <c r="L14" s="30">
@@ -3154,11 +3176,11 @@
         <v>65.181544400162522</v>
       </c>
       <c r="N14" s="19">
-        <f>[13]Main!$N$4</f>
+        <f>[14]Main!$N$4</f>
         <v>75.75</v>
       </c>
       <c r="O14" s="19">
-        <f>[13]Main!$N$13</f>
+        <f>[14]Main!$N$13</f>
         <v>69.464871001991241</v>
       </c>
       <c r="P14" s="32">
@@ -3189,19 +3211,19 @@
         <v>115</v>
       </c>
       <c r="H15" s="12">
-        <f>[14]Main!$N$9</f>
+        <f>[15]Main!$N$9</f>
         <v>43973.122093023252</v>
       </c>
       <c r="I15" s="13">
-        <f>+[14]Main!$N$6</f>
+        <f>+[15]Main!$N$6</f>
         <v>14394.122093023256</v>
       </c>
       <c r="J15" s="13">
-        <f>[14]Main!$N$12</f>
+        <f>[15]Main!$N$12</f>
         <v>18848.439289507303</v>
       </c>
       <c r="K15" s="13">
-        <f>+[14]Model!$Z$27</f>
+        <f>+[15]Model!$Z$27</f>
         <v>-2103</v>
       </c>
       <c r="L15" s="30">
@@ -3213,11 +3235,11 @@
         <v>-20.909710933439491</v>
       </c>
       <c r="N15" s="19">
-        <f>[14]Main!$N$4</f>
+        <f>[15]Main!$N$4</f>
         <v>12.19</v>
       </c>
       <c r="O15" s="19">
-        <f>[14]Main!$N$13</f>
+        <f>[15]Main!$N$13</f>
         <v>15.962243022133215</v>
       </c>
       <c r="P15" s="32">
@@ -3233,7 +3255,7 @@
         <v>120</v>
       </c>
       <c r="C16" s="4">
-        <f>+[15]Main!$N$2</f>
+        <f>+[16]Main!$N$2</f>
         <v>44985</v>
       </c>
       <c r="D16" s="28">
@@ -3249,19 +3271,19 @@
         <v>117</v>
       </c>
       <c r="H16" s="12">
-        <f>[15]Main!$N$9</f>
+        <f>[16]Main!$N$9</f>
         <v>18224.220440000001</v>
       </c>
       <c r="I16" s="13">
-        <f>+[15]Main!$N$6</f>
+        <f>+[16]Main!$N$6</f>
         <v>5320.9374400000006</v>
       </c>
       <c r="J16" s="13">
-        <f>[15]Main!$N$12</f>
+        <f>[16]Main!$N$12</f>
         <v>9564.1035156825055</v>
       </c>
       <c r="K16" s="13">
-        <f>+SUM([15]Model!$G$26:$J$26)</f>
+        <f>+SUM([16]Model!$G$26:$J$26)</f>
         <v>-802.42000000000019</v>
       </c>
       <c r="L16" s="30">
@@ -3273,11 +3295,11 @@
         <v>-22.711573041549308</v>
       </c>
       <c r="N16" s="19">
-        <f>[15]Main!$N$4</f>
+        <f>[16]Main!$N$4</f>
         <v>14.56</v>
       </c>
       <c r="O16" s="19">
-        <f>[15]Main!$N$13</f>
+        <f>[16]Main!$N$13</f>
         <v>26.170829625152908</v>
       </c>
       <c r="P16" s="32">
@@ -3308,15 +3330,15 @@
         <v>118</v>
       </c>
       <c r="H17" s="12">
-        <f>[16]Main!$N$9</f>
+        <f>[17]Main!$N$9</f>
         <v>1089.1226000000001</v>
       </c>
       <c r="I17" s="13">
-        <f>+[16]Main!$N$6</f>
+        <f>+[17]Main!$N$6</f>
         <v>619.56560000000002</v>
       </c>
       <c r="J17" s="13">
-        <f>[16]Main!$N$12</f>
+        <f>[17]Main!$N$12</f>
         <v>473.84250172820322</v>
       </c>
       <c r="K17" s="13">
@@ -3331,11 +3353,11 @@
         <v>544.56130000000007</v>
       </c>
       <c r="N17" s="19">
-        <f>[16]Main!$N$4</f>
+        <f>[17]Main!$N$4</f>
         <v>11.68</v>
       </c>
       <c r="O17" s="19">
-        <f>[16]Main!$N$13</f>
+        <f>[17]Main!$N$13</f>
         <v>8.932840074054166</v>
       </c>
       <c r="P17" s="32">
@@ -3366,19 +3388,19 @@
         <v>21</v>
       </c>
       <c r="H18" s="12">
-        <f>[17]Main!$N$10</f>
+        <f>[18]Main!$N$10</f>
         <v>156055.80000000002</v>
       </c>
       <c r="I18" s="13">
-        <f>+[17]Main!$N$7</f>
+        <f>+[18]Main!$N$7</f>
         <v>155536.80000000002</v>
       </c>
       <c r="J18" s="13">
-        <f>[17]Main!$N$12</f>
+        <f>[18]Main!$N$12</f>
         <v>134489.60313830531</v>
       </c>
       <c r="K18" s="13">
-        <f>[17]Model!$X$28</f>
+        <f>[18]Model!$X$28</f>
         <v>11119</v>
       </c>
       <c r="L18" s="30">
@@ -3390,11 +3412,11 @@
         <v>14.035057109452291</v>
       </c>
       <c r="N18" s="19">
-        <f>[17]Main!$N$5</f>
+        <f>[18]Main!$N$5</f>
         <v>169.8</v>
       </c>
       <c r="O18" s="19">
-        <f>[17]Main!$N$13</f>
+        <f>[18]Main!$N$13</f>
         <v>146.82271084967829</v>
       </c>
       <c r="P18" s="32">
@@ -3428,19 +3450,19 @@
         <v>20</v>
       </c>
       <c r="H19" s="12">
-        <f>[18]Main!$N$10</f>
+        <f>[19]Main!$N$10</f>
         <v>99554.828000000009</v>
       </c>
       <c r="I19" s="13">
-        <f>+[18]Main!$N$7</f>
+        <f>+[19]Main!$N$7</f>
         <v>94146.828000000009</v>
       </c>
       <c r="J19" s="13">
-        <f>+[18]Main!$N$13</f>
+        <f>+[19]Main!$N$13</f>
         <v>95545.612738294119</v>
       </c>
       <c r="K19" s="13">
-        <f>SUM([18]Model!$J$29:$M$29)</f>
+        <f>SUM([19]Model!$J$29:$M$29)</f>
         <v>1530.8109999999983</v>
       </c>
       <c r="L19" s="30">
@@ -3452,11 +3474,11 @@
         <v>65.034042739436885</v>
       </c>
       <c r="N19" s="19">
-        <f>+[18]Main!$N$5</f>
+        <f>+[19]Main!$N$5</f>
         <v>185.65</v>
       </c>
       <c r="O19" s="19">
-        <f>+[18]Main!$N$14</f>
+        <f>+[19]Main!$N$14</f>
         <v>188.40829140695323</v>
       </c>
       <c r="P19" s="32">
@@ -3490,19 +3512,19 @@
         <v>127</v>
       </c>
       <c r="H20" s="12">
-        <f>+[19]Main!$N$12</f>
+        <f>+[20]Main!$N$12</f>
         <v>34171.095999999998</v>
       </c>
       <c r="I20" s="13">
-        <f>+[19]Main!$N$9</f>
+        <f>+[20]Main!$N$9</f>
         <v>33044.495999999999</v>
       </c>
       <c r="J20" s="13">
-        <f>+[19]Main!$N$15</f>
+        <f>+[20]Main!$N$15</f>
         <v>35110.668973847663</v>
       </c>
       <c r="K20" s="13">
-        <f>+[19]Model!$X$29</f>
+        <f>+[20]Model!$X$29</f>
         <v>2922.8000000000011</v>
       </c>
       <c r="L20" s="30">
@@ -3514,11 +3536,11 @@
         <v>11.691219378677975</v>
       </c>
       <c r="N20" s="19">
-        <f>+[19]Main!$N$7</f>
+        <f>+[20]Main!$N$7</f>
         <v>76.28</v>
       </c>
       <c r="O20" s="19">
-        <f>+[19]Main!$N$16</f>
+        <f>+[20]Main!$N$16</f>
         <v>81.049559034736063</v>
       </c>
       <c r="P20" s="32">
@@ -3552,19 +3574,19 @@
         <v>131</v>
       </c>
       <c r="H21" s="12">
-        <f>+[20]Main!$N$11</f>
+        <f>+[21]Main!$N$11</f>
         <v>50060.056000000004</v>
       </c>
       <c r="I21" s="13">
-        <f>+[20]Main!$N$8</f>
+        <f>+[21]Main!$N$8</f>
         <v>43760.256000000008</v>
       </c>
       <c r="J21" s="13">
-        <f>+[20]Main!$N$14</f>
+        <f>+[21]Main!$N$14</f>
         <v>49396.022818172591</v>
       </c>
       <c r="K21" s="13">
-        <f>+SUM([20]Model!$F$28:$I$28)</f>
+        <f>+SUM([21]Model!$F$28:$I$28)</f>
         <v>3890.6999999999989</v>
       </c>
       <c r="L21" s="30">
@@ -3576,11 +3598,11 @@
         <v>12.866593672089859</v>
       </c>
       <c r="N21" s="19">
-        <f>+[20]Main!$N$6</f>
+        <f>+[21]Main!$N$6</f>
         <v>79.680000000000007</v>
       </c>
       <c r="O21" s="19">
-        <f>+[20]Main!$N$15</f>
+        <f>+[21]Main!$N$15</f>
         <v>89.941774978464281</v>
       </c>
       <c r="P21" s="32">
@@ -3614,19 +3636,19 @@
         <v>134</v>
       </c>
       <c r="H22" s="12">
-        <f>+[21]Main!$N$11</f>
+        <f>+[22]Main!$N$11</f>
         <v>1828.46028</v>
       </c>
       <c r="I22" s="13">
-        <f>+[21]Main!$N$8</f>
+        <f>+[22]Main!$N$8</f>
         <v>1946.07728</v>
       </c>
       <c r="J22" s="13">
-        <f>+[21]Main!$N$14</f>
+        <f>+[22]Main!$N$14</f>
         <v>2173.7463596759726</v>
       </c>
       <c r="K22" s="13">
-        <f>SUM([21]Model!$F$28:$I$28)</f>
+        <f>SUM([22]Model!$F$28:$I$28)</f>
         <v>226.52699999999987</v>
       </c>
       <c r="L22" s="30">
@@ -3638,11 +3660,11 @@
         <v>8.0717101272696024</v>
       </c>
       <c r="N22" s="19">
-        <f>+[21]Main!$N$6</f>
+        <f>+[22]Main!$N$6</f>
         <v>30.52</v>
       </c>
       <c r="O22" s="19">
-        <f>+[21]Main!$N$15</f>
+        <f>+[22]Main!$N$15</f>
         <v>34.090495572360147</v>
       </c>
       <c r="P22" s="32">
@@ -3673,23 +3695,23 @@
         <v>142</v>
       </c>
       <c r="G23" t="str">
-        <f>+[22]Main!$N$4</f>
+        <f>+[23]Main!$N$4</f>
         <v>Old Dominion Freight Line</v>
       </c>
       <c r="H23" s="12">
-        <f>+[22]Main!$N$11</f>
+        <f>+[23]Main!$N$11</f>
         <v>39621.008000000002</v>
       </c>
       <c r="I23" s="13">
-        <f>+[22]Main!$N$8</f>
+        <f>+[23]Main!$N$8</f>
         <v>39650.402999999998</v>
       </c>
       <c r="J23" s="13">
-        <f>+[22]Main!$N$14</f>
+        <f>+[23]Main!$N$14</f>
         <v>34330.520064169796</v>
       </c>
       <c r="K23" s="13">
-        <f>+[22]Model!$T$32</f>
+        <f>+[23]Model!$T$32</f>
         <v>2116.6350000000002</v>
       </c>
       <c r="L23" s="30">
@@ -3701,11 +3723,11 @@
         <v>18.718866502727206</v>
       </c>
       <c r="N23" s="19">
-        <f>+[22]Main!$N$6</f>
+        <f>+[23]Main!$N$6</f>
         <v>352.95</v>
       </c>
       <c r="O23" s="19">
-        <f>+[22]Main!$N$15</f>
+        <f>+[23]Main!$N$15</f>
         <v>305.59480206667075</v>
       </c>
       <c r="P23" s="32">
@@ -3724,11 +3746,11 @@
         <v>141</v>
       </c>
       <c r="C24" s="4">
-        <f>+[23]Main!$N$2</f>
+        <f>+[24]Main!$N$2</f>
         <v>44992</v>
       </c>
       <c r="D24" s="28">
-        <f>+[23]Model!$J$1</f>
+        <f>+[24]Model!$J$1</f>
         <v>44595</v>
       </c>
       <c r="E24" t="s">
@@ -3738,23 +3760,23 @@
         <v>143</v>
       </c>
       <c r="G24" t="str">
-        <f>+[23]Main!$N$4</f>
+        <f>+[24]Main!$N$4</f>
         <v>Saia</v>
       </c>
       <c r="H24" s="12">
-        <f>+[23]Main!$N$11</f>
+        <f>+[24]Main!$N$11</f>
         <v>7707.5203999999994</v>
       </c>
       <c r="I24" s="13">
-        <f>+[23]Main!$N$8</f>
+        <f>+[24]Main!$N$8</f>
         <v>7658.1803999999993</v>
       </c>
       <c r="J24" s="13">
-        <f>+[23]Main!$N$14</f>
+        <f>+[24]Main!$N$14</f>
         <v>7684.7281871497207</v>
       </c>
       <c r="K24" s="13">
-        <f>+[23]Model!$T$28</f>
+        <f>+[24]Model!$T$28</f>
         <v>627.74999999999977</v>
       </c>
       <c r="L24" s="30">
@@ -3766,11 +3788,11 @@
         <v>12.278009398645962</v>
       </c>
       <c r="N24" s="19">
-        <f>+[23]Main!$N$6</f>
+        <f>+[24]Main!$N$6</f>
         <v>288.77</v>
       </c>
       <c r="O24" s="19">
-        <f>+[23]Main!$N$15</f>
+        <f>+[24]Main!$N$15</f>
         <v>289.77104778090956</v>
       </c>
       <c r="P24" s="32">
@@ -3789,11 +3811,11 @@
         <v>141</v>
       </c>
       <c r="C25" s="4">
-        <f>+[24]Main!$N$2</f>
+        <f>+[25]Main!$N$2</f>
         <v>44992</v>
       </c>
       <c r="D25" s="28">
-        <f>+[24]Model!$J$1</f>
+        <f>+[25]Model!$J$1</f>
         <v>44605</v>
       </c>
       <c r="E25" t="s">
@@ -3803,23 +3825,23 @@
         <v>144</v>
       </c>
       <c r="G25" t="str">
-        <f>+[24]Main!$N$4</f>
+        <f>+[25]Main!$N$4</f>
         <v>P.A.M. Transportation Services</v>
       </c>
       <c r="H25" s="12">
-        <f>+[24]Main!$N$11</f>
+        <f>+[25]Main!$N$11</f>
         <v>853.44364000000007</v>
       </c>
       <c r="I25" s="13">
-        <f>+[24]Main!$N$8</f>
+        <f>+[25]Main!$N$8</f>
         <v>656.02864</v>
       </c>
       <c r="J25" s="13">
-        <f>+[24]Main!$N$14</f>
+        <f>+[25]Main!$N$14</f>
         <v>970.90412687107221</v>
       </c>
       <c r="K25" s="13">
-        <f>+[24]Model!$T$31</f>
+        <f>+[25]Model!$T$31</f>
         <v>186.68</v>
       </c>
       <c r="L25" s="30">
@@ -3831,11 +3853,11 @@
         <v>4.571692950503536</v>
       </c>
       <c r="N25" s="19">
-        <f>+[24]Main!$N$6</f>
+        <f>+[25]Main!$N$6</f>
         <v>29.24</v>
       </c>
       <c r="O25" s="19">
-        <f>+[24]Main!$N$15</f>
+        <f>+[25]Main!$N$15</f>
         <v>43.274386114774124</v>
       </c>
       <c r="P25" s="32">
@@ -3854,58 +3876,58 @@
         <v>141</v>
       </c>
       <c r="C26" s="4">
-        <f>+[25]Main!$N$2</f>
-        <v>44992</v>
+        <f>+[26]Main!$N$2</f>
+        <v>45047</v>
       </c>
       <c r="D26" s="28">
-        <f>+[25]Model!$J$1</f>
-        <v>44951</v>
+        <f>+[26]Model!$K$1</f>
+        <v>45044</v>
       </c>
       <c r="E26" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F26" s="26" t="s">
         <v>147</v>
       </c>
       <c r="G26" t="str">
-        <f>+[25]Main!$N$4</f>
+        <f>+[26]Main!$N$4</f>
         <v>Covenant Logistics Group</v>
       </c>
       <c r="H26" s="12">
-        <f>+[25]Main!$N$11</f>
-        <v>635.8222199999999</v>
+        <f>+[26]Main!$N$11</f>
+        <v>628.53698000000009</v>
       </c>
       <c r="I26" s="13">
-        <f>+[25]Main!$N$8</f>
-        <v>530.76221999999996</v>
+        <f>+[26]Main!$N$8</f>
+        <v>563.56698000000006</v>
       </c>
       <c r="J26" s="13">
-        <f>+[25]Main!$N$14</f>
-        <v>675.0558523176453</v>
+        <f>+[26]Main!$N$14</f>
+        <v>546.57156432801094</v>
       </c>
       <c r="K26" s="13">
-        <f>+[25]Model!$T$35</f>
+        <f>+[26]Model!$U$35</f>
         <v>178.19999999999982</v>
       </c>
       <c r="L26" s="30">
         <f t="shared" si="1"/>
-        <v>11.875249900039972</v>
+        <v>13.337325050520157</v>
       </c>
       <c r="M26" s="31">
         <f>H26/K26</f>
-        <v>3.5680259259259288</v>
+        <v>3.5271435465768839</v>
       </c>
       <c r="N26" s="19">
-        <f>+[25]Main!$N$6</f>
-        <v>35.369999999999997</v>
+        <f>+[26]Main!$N$6</f>
+        <v>42.18</v>
       </c>
       <c r="O26" s="19">
-        <f>+[25]Main!$N$15</f>
-        <v>44.985729196164556</v>
+        <f>+[26]Main!$N$15</f>
+        <v>40.907983259337691</v>
       </c>
       <c r="P26" s="32">
         <f t="shared" si="3"/>
-        <v>1.2718611590660038</v>
+        <v>0.9698431308520078</v>
       </c>
       <c r="Q26" t="s">
         <v>149</v>
@@ -3919,11 +3941,11 @@
         <v>141</v>
       </c>
       <c r="C27" s="4">
-        <f>+[26]Main!$N$2</f>
+        <f>+[27]Main!$N$2</f>
         <v>44993</v>
       </c>
       <c r="D27" s="28">
-        <f>+[26]Model!$J$1</f>
+        <f>+[27]Model!$J$1</f>
         <v>44595</v>
       </c>
       <c r="E27" t="s">
@@ -3933,23 +3955,23 @@
         <v>150</v>
       </c>
       <c r="G27" t="str">
-        <f>+[26]Main!$N$4</f>
+        <f>+[27]Main!$N$4</f>
         <v>Heartland Express</v>
       </c>
       <c r="H27" s="12">
-        <f>+[26]Main!$N$11</f>
+        <f>+[27]Main!$N$11</f>
         <v>1763.72066</v>
       </c>
       <c r="I27" s="13">
-        <f>+[26]Main!$N$8</f>
+        <f>+[27]Main!$N$8</f>
         <v>1283.5806600000001</v>
       </c>
       <c r="J27" s="13">
-        <f>+[26]Main!$N$14</f>
+        <f>+[27]Main!$N$14</f>
         <v>1294.1990734380452</v>
       </c>
       <c r="K27" s="13">
-        <f>+[26]Main!$N$17</f>
+        <f>+[27]Main!$N$17</f>
         <v>321.39600000000002</v>
       </c>
       <c r="L27" s="30">
@@ -3961,11 +3983,11 @@
         <v>5.4876870278410435</v>
       </c>
       <c r="N27" s="19">
-        <f>+[26]Main!$N$6</f>
+        <f>+[27]Main!$N$6</f>
         <v>16.260000000000002</v>
       </c>
       <c r="O27" s="19">
-        <f>+[26]Main!$N$15</f>
+        <f>+[27]Main!$N$15</f>
         <v>16.394510754082734</v>
       </c>
       <c r="P27" s="32">
@@ -3984,11 +4006,11 @@
         <v>141</v>
       </c>
       <c r="C28" s="4">
-        <f>+[27]Main!$N$2</f>
+        <f>+[28]Main!$N$2</f>
         <v>44993</v>
       </c>
       <c r="D28" s="28">
-        <f>+[27]Model!$J$1</f>
+        <f>+[28]Model!$J$1</f>
         <v>0</v>
       </c>
       <c r="E28" t="s">
@@ -3998,23 +4020,23 @@
         <v>151</v>
       </c>
       <c r="G28" t="str">
-        <f>+[27]Main!$N$4</f>
+        <f>+[28]Main!$N$4</f>
         <v>ArcBest Corporation</v>
       </c>
       <c r="H28" s="12">
-        <f>+[27]Main!$N$11</f>
+        <f>+[28]Main!$N$11</f>
         <v>2754.4777000000004</v>
       </c>
       <c r="I28" s="13">
-        <f>+[27]Main!$N$8</f>
+        <f>+[28]Main!$N$8</f>
         <v>2498.3277000000003</v>
       </c>
       <c r="J28" s="13">
-        <f>+[27]Main!$N$14</f>
+        <f>+[28]Main!$N$14</f>
         <v>3083.7037867156318</v>
       </c>
       <c r="K28" s="13">
-        <f>+[27]Main!$N$17</f>
+        <f>+[28]Main!$N$17</f>
         <v>539.48500000000149</v>
       </c>
       <c r="L28" s="30">
@@ -4026,11 +4048,11 @@
         <v>5.1057540061354674</v>
       </c>
       <c r="N28" s="19">
-        <f>+[27]Main!$N$6</f>
+        <f>+[28]Main!$N$6</f>
         <v>101.62</v>
       </c>
       <c r="O28" s="19">
-        <f>+[27]Main!$N$15</f>
+        <f>+[28]Main!$N$15</f>
         <v>125.4302943549169</v>
       </c>
       <c r="P28" s="32">
@@ -4257,8 +4279,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K1048576 K1">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="K2">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4269,8 +4291,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K3:K1048576 K1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4463,19 +4485,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="12">
-        <f>+[28]Main!$J$8</f>
+        <f>+[29]Main!$J$8</f>
         <v>87517.207200000004</v>
       </c>
       <c r="H6" s="13">
-        <f>+[28]Main!$J$18</f>
+        <f>+[29]Main!$J$18</f>
         <v>74903.518611460153</v>
       </c>
       <c r="I6" s="23">
-        <f>+[28]Main!$J$3</f>
+        <f>+[29]Main!$J$3</f>
         <v>67.2</v>
       </c>
       <c r="J6" s="23">
-        <f>+[28]Main!$J$19</f>
+        <f>+[29]Main!$J$19</f>
         <v>63.631730278242067</v>
       </c>
       <c r="K6" s="14">
@@ -4587,6 +4609,18 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -4599,20 +4633,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K1048576 K5">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="K1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4635,8 +4657,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="K6">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4647,8 +4669,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K7:K1048576 K5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4758,19 +4780,19 @@
         <v>93</v>
       </c>
       <c r="G2" s="12">
-        <f>[29]Main!$O$8</f>
+        <f>[30]Main!$O$8</f>
         <v>506.71814999999992</v>
       </c>
       <c r="H2" s="13">
-        <f>[29]Main!$O$18</f>
+        <f>[30]Main!$O$18</f>
         <v>541.46267091390234</v>
       </c>
       <c r="I2" s="23">
-        <f>[29]Main!$O$3</f>
+        <f>[30]Main!$O$3</f>
         <v>18.149999999999999</v>
       </c>
       <c r="J2" s="24">
-        <f>[29]Main!$O$19</f>
+        <f>[30]Main!$O$19</f>
         <v>16.629178185986376</v>
       </c>
       <c r="K2" s="14">
@@ -4798,19 +4820,19 @@
         <v>99</v>
       </c>
       <c r="G3" s="12">
-        <f>+[30]Main!$N$8</f>
+        <f>+[31]Main!$N$8</f>
         <v>217.09325999999999</v>
       </c>
       <c r="H3" s="13">
-        <f>+[30]Main!$N$18</f>
+        <f>+[31]Main!$N$18</f>
         <v>42.225188935657137</v>
       </c>
       <c r="I3" s="19">
-        <f>+[30]Main!$N$3</f>
+        <f>+[31]Main!$N$3</f>
         <v>4.43</v>
       </c>
       <c r="J3" s="25">
-        <f>+[30]Main!$N$19</f>
+        <f>+[31]Main!$N$19</f>
         <v>0.9450156424434254</v>
       </c>
       <c r="K3" s="14">
@@ -4841,19 +4863,19 @@
         <v>104</v>
       </c>
       <c r="G4" s="12">
-        <f>[31]Main!$J$8</f>
+        <f>[32]Main!$J$8</f>
         <v>3802.98</v>
       </c>
       <c r="H4" s="13">
-        <f>[31]Main!$J$18</f>
+        <f>[32]Main!$J$18</f>
         <v>218.76521315251679</v>
       </c>
       <c r="I4" s="23">
-        <f>[31]Main!$J$3</f>
+        <f>[32]Main!$J$3</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="J4" s="25">
-        <f>[31]Main!$J$19</f>
+        <f>[32]Main!$J$19</f>
         <v>2.7483066978959396</v>
       </c>
       <c r="K4" s="14">
@@ -4921,8 +4943,8 @@
       <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="E1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4933,20 +4955,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4981,6 +4991,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2BA61AB2-B324-4A96-BC09-D9608FDE949E}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{1252D7D6-1977-4A37-ADFC-E3118CFC39F8}"/>

</xml_diff>